<commit_message>
2025 02 03 17:00
</commit_message>
<xml_diff>
--- a/2팀(Pick+Course)보고양식.xlsx
+++ b/2팀(Pick+Course)보고양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gb_0900_jdy\git\workspace\pickcourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E3C175-A07B-4556-BE79-B2D53E4D7F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E752C052-89A0-41A2-8E38-288A58DFEEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -268,10 +268,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>조승찬</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>봉사 코스</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -312,8 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
   <fonts count="7">
@@ -461,7 +456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -471,11 +466,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -509,15 +501,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -536,19 +519,18 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
-    <cellStyle name="쉼표 [0]" xfId="3" builtinId="6"/>
     <cellStyle name="좋음" xfId="2" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -950,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1071,15 +1053,15 @@
       </c>
       <c r="G3" s="6">
         <f t="shared" si="0"/>
-        <v>3.3333333333333333E-2</v>
+        <v>8.3333333333333343E-2</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" si="0"/>
-        <v>0.21583333333333332</v>
+        <v>0.26583333333333331</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" si="0"/>
@@ -1280,10 +1262,10 @@
       </c>
     </row>
     <row r="6" spans="2:34">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1379,8 +1361,8 @@
       </c>
     </row>
     <row r="7" spans="2:34">
-      <c r="B7" s="15"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="7" t="s">
         <v>52</v>
       </c>
@@ -1474,8 +1456,8 @@
       </c>
     </row>
     <row r="8" spans="2:34">
-      <c r="B8" s="15"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1569,8 +1551,8 @@
       </c>
     </row>
     <row r="9" spans="2:34">
-      <c r="B9" s="15"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1664,8 +1646,8 @@
       </c>
     </row>
     <row r="10" spans="2:34">
-      <c r="B10" s="15"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1759,8 +1741,8 @@
       </c>
     </row>
     <row r="11" spans="2:34">
-      <c r="B11" s="15"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1854,8 +1836,8 @@
       </c>
     </row>
     <row r="12" spans="2:34">
-      <c r="B12" s="15"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1949,8 +1931,8 @@
       </c>
     </row>
     <row r="13" spans="2:34">
-      <c r="B13" s="15"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
@@ -2044,8 +2026,8 @@
       </c>
     </row>
     <row r="14" spans="2:34">
-      <c r="B14" s="15"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2139,8 +2121,8 @@
       </c>
     </row>
     <row r="15" spans="2:34">
-      <c r="B15" s="15"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
@@ -2234,8 +2216,8 @@
       </c>
     </row>
     <row r="16" spans="2:34">
-      <c r="B16" s="15"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="7" t="s">
         <v>14</v>
       </c>
@@ -2329,8 +2311,8 @@
       </c>
     </row>
     <row r="17" spans="2:34">
-      <c r="B17" s="15"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
@@ -2424,8 +2406,8 @@
       </c>
     </row>
     <row r="18" spans="2:34">
-      <c r="B18" s="15"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="7" t="s">
         <v>16</v>
       </c>
@@ -2519,8 +2501,8 @@
       </c>
     </row>
     <row r="19" spans="2:34">
-      <c r="B19" s="15"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="7" t="s">
         <v>17</v>
       </c>
@@ -2614,8 +2596,8 @@
       </c>
     </row>
     <row r="20" spans="2:34">
-      <c r="B20" s="15"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="7" t="s">
         <v>18</v>
       </c>
@@ -2709,8 +2691,8 @@
       </c>
     </row>
     <row r="21" spans="2:34" ht="16.149999999999999" customHeight="1">
-      <c r="B21" s="16"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="6">
@@ -2831,10 +2813,8 @@
       </c>
     </row>
     <row r="22" spans="2:34">
-      <c r="B22" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="12"/>
+      <c r="C22" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D22" s="7" t="s">
@@ -2930,8 +2910,8 @@
       </c>
     </row>
     <row r="23" spans="2:34">
-      <c r="B23" s="21"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="7" t="s">
         <v>24</v>
       </c>
@@ -3025,8 +3005,8 @@
       </c>
     </row>
     <row r="24" spans="2:34">
-      <c r="B24" s="21"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="7" t="s">
         <v>25</v>
       </c>
@@ -3120,8 +3100,8 @@
       </c>
     </row>
     <row r="25" spans="2:34">
-      <c r="B25" s="21"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="7" t="s">
         <v>26</v>
       </c>
@@ -3215,8 +3195,8 @@
       </c>
     </row>
     <row r="26" spans="2:34">
-      <c r="B26" s="22"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="6">
@@ -3337,10 +3317,8 @@
       </c>
     </row>
     <row r="27" spans="2:34">
-      <c r="B27" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="17" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -3436,8 +3414,8 @@
       </c>
     </row>
     <row r="28" spans="2:34">
-      <c r="B28" s="15"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="7" t="s">
         <v>3</v>
       </c>
@@ -3531,8 +3509,8 @@
       </c>
     </row>
     <row r="29" spans="2:34">
-      <c r="B29" s="15"/>
-      <c r="C29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
@@ -3626,8 +3604,8 @@
       </c>
     </row>
     <row r="30" spans="2:34">
-      <c r="B30" s="15"/>
-      <c r="C30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="7" t="s">
         <v>21</v>
       </c>
@@ -3721,8 +3699,8 @@
       </c>
     </row>
     <row r="31" spans="2:34">
-      <c r="B31" s="15"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="7" t="s">
         <v>22</v>
       </c>
@@ -3816,8 +3794,8 @@
       </c>
     </row>
     <row r="32" spans="2:34">
-      <c r="B32" s="15"/>
-      <c r="C32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="7" t="s">
         <v>23</v>
       </c>
@@ -3911,8 +3889,8 @@
       </c>
     </row>
     <row r="33" spans="2:34">
-      <c r="B33" s="16"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="6">
@@ -4033,10 +4011,10 @@
       </c>
     </row>
     <row r="34" spans="2:34">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="14" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
@@ -4132,8 +4110,8 @@
       </c>
     </row>
     <row r="35" spans="2:34">
-      <c r="B35" s="15"/>
-      <c r="C35" s="18"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="7" t="s">
         <v>54</v>
       </c>
@@ -4227,10 +4205,10 @@
       </c>
     </row>
     <row r="36" spans="2:34">
-      <c r="B36" s="15"/>
-      <c r="C36" s="18"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="9">
@@ -4322,8 +4300,8 @@
       </c>
     </row>
     <row r="37" spans="2:34">
-      <c r="B37" s="15"/>
-      <c r="C37" s="18"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="15"/>
       <c r="D37" s="7" t="s">
         <v>55</v>
       </c>
@@ -4417,8 +4395,8 @@
       </c>
     </row>
     <row r="38" spans="2:34">
-      <c r="B38" s="15"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="10" t="s">
         <v>56</v>
       </c>
@@ -4512,8 +4490,8 @@
       </c>
     </row>
     <row r="39" spans="2:34">
-      <c r="B39" s="15"/>
-      <c r="C39" s="18"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="10" t="s">
         <v>57</v>
       </c>
@@ -4607,10 +4585,10 @@
       </c>
     </row>
     <row r="40" spans="2:34">
-      <c r="B40" s="15"/>
-      <c r="C40" s="18"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="15"/>
       <c r="D40" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="9">
@@ -4702,10 +4680,10 @@
       </c>
     </row>
     <row r="41" spans="2:34">
-      <c r="B41" s="15"/>
-      <c r="C41" s="18"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="15"/>
       <c r="D41" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="9">
@@ -4797,8 +4775,8 @@
       </c>
     </row>
     <row r="42" spans="2:34">
-      <c r="B42" s="16"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="6">
@@ -4919,14 +4897,12 @@
       </c>
     </row>
     <row r="43" spans="2:34">
-      <c r="B43" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="17" t="s">
+      <c r="B43" s="12"/>
+      <c r="C43" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="9">
@@ -5018,10 +4994,10 @@
       </c>
     </row>
     <row r="44" spans="2:34">
-      <c r="B44" s="15"/>
-      <c r="C44" s="18"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="9">
@@ -5113,10 +5089,10 @@
       </c>
     </row>
     <row r="45" spans="2:34">
-      <c r="B45" s="15"/>
-      <c r="C45" s="18"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="15"/>
       <c r="D45" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="9">
@@ -5208,8 +5184,8 @@
       </c>
     </row>
     <row r="46" spans="2:34">
-      <c r="B46" s="15"/>
-      <c r="C46" s="18"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="7" t="s">
         <v>53</v>
       </c>
@@ -5303,10 +5279,10 @@
       </c>
     </row>
     <row r="47" spans="2:34">
-      <c r="B47" s="15"/>
-      <c r="C47" s="18"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="9">
@@ -5398,10 +5374,10 @@
       </c>
     </row>
     <row r="48" spans="2:34">
-      <c r="B48" s="15"/>
-      <c r="C48" s="18"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="9">
@@ -5493,8 +5469,8 @@
       </c>
     </row>
     <row r="49" spans="2:34">
-      <c r="B49" s="15"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="15"/>
       <c r="D49" s="7" t="s">
         <v>16</v>
       </c>
@@ -5588,8 +5564,8 @@
       </c>
     </row>
     <row r="50" spans="2:34">
-      <c r="B50" s="16"/>
-      <c r="C50" s="19"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="6">
@@ -5710,11 +5686,9 @@
       </c>
     </row>
     <row r="51" spans="2:34">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="12"/>
+      <c r="C51" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>59</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>32</v>
@@ -5809,8 +5783,8 @@
       </c>
     </row>
     <row r="52" spans="2:34">
-      <c r="B52" s="15"/>
-      <c r="C52" s="18"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="15"/>
       <c r="D52" s="7" t="s">
         <v>53</v>
       </c>
@@ -5904,8 +5878,8 @@
       </c>
     </row>
     <row r="53" spans="2:34">
-      <c r="B53" s="16"/>
-      <c r="C53" s="19"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="6">
@@ -6026,10 +6000,10 @@
       </c>
     </row>
     <row r="54" spans="2:34">
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="7" t="s">
@@ -6125,8 +6099,8 @@
       </c>
     </row>
     <row r="55" spans="2:34">
-      <c r="B55" s="15"/>
-      <c r="C55" s="18"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="15"/>
       <c r="D55" s="7" t="s">
         <v>36</v>
       </c>
@@ -6220,8 +6194,8 @@
       </c>
     </row>
     <row r="56" spans="2:34">
-      <c r="B56" s="15"/>
-      <c r="C56" s="18"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="15"/>
       <c r="D56" s="7" t="s">
         <v>37</v>
       </c>
@@ -6315,8 +6289,8 @@
       </c>
     </row>
     <row r="57" spans="2:34">
-      <c r="B57" s="15"/>
-      <c r="C57" s="18"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="15"/>
       <c r="D57" s="7" t="s">
         <v>25</v>
       </c>
@@ -6410,8 +6384,8 @@
       </c>
     </row>
     <row r="58" spans="2:34">
-      <c r="B58" s="15"/>
-      <c r="C58" s="18"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="15"/>
       <c r="D58" s="7" t="s">
         <v>26</v>
       </c>
@@ -6505,8 +6479,8 @@
       </c>
     </row>
     <row r="59" spans="2:34">
-      <c r="B59" s="15"/>
-      <c r="C59" s="18"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="15"/>
       <c r="D59" s="7" t="s">
         <v>38</v>
       </c>
@@ -6600,8 +6574,8 @@
       </c>
     </row>
     <row r="60" spans="2:34">
-      <c r="B60" s="15"/>
-      <c r="C60" s="18"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="15"/>
       <c r="D60" s="7" t="s">
         <v>39</v>
       </c>
@@ -6695,8 +6669,8 @@
       </c>
     </row>
     <row r="61" spans="2:34">
-      <c r="B61" s="15"/>
-      <c r="C61" s="18"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="15"/>
       <c r="D61" s="7" t="s">
         <v>7</v>
       </c>
@@ -6790,8 +6764,8 @@
       </c>
     </row>
     <row r="62" spans="2:34">
-      <c r="B62" s="15"/>
-      <c r="C62" s="18"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="15"/>
       <c r="D62" s="7" t="s">
         <v>8</v>
       </c>
@@ -6885,8 +6859,8 @@
       </c>
     </row>
     <row r="63" spans="2:34">
-      <c r="B63" s="15"/>
-      <c r="C63" s="18"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="15"/>
       <c r="D63" s="7" t="s">
         <v>40</v>
       </c>
@@ -6980,8 +6954,8 @@
       </c>
     </row>
     <row r="64" spans="2:34">
-      <c r="B64" s="15"/>
-      <c r="C64" s="18"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="15"/>
       <c r="D64" s="7" t="s">
         <v>41</v>
       </c>
@@ -7075,8 +7049,8 @@
       </c>
     </row>
     <row r="65" spans="2:34">
-      <c r="B65" s="15"/>
-      <c r="C65" s="18"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="15"/>
       <c r="D65" s="7" t="s">
         <v>42</v>
       </c>
@@ -7170,8 +7144,8 @@
       </c>
     </row>
     <row r="66" spans="2:34">
-      <c r="B66" s="15"/>
-      <c r="C66" s="18"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="15"/>
       <c r="D66" s="7" t="s">
         <v>43</v>
       </c>
@@ -7265,8 +7239,8 @@
       </c>
     </row>
     <row r="67" spans="2:34">
-      <c r="B67" s="16"/>
-      <c r="C67" s="19"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="16"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="6">
@@ -7387,10 +7361,8 @@
       </c>
     </row>
     <row r="68" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B68" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" s="11" t="s">
+      <c r="B68" s="12"/>
+      <c r="C68" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D68" s="7" t="s">
@@ -7486,8 +7458,8 @@
       </c>
     </row>
     <row r="69" spans="2:34">
-      <c r="B69" s="16"/>
-      <c r="C69" s="13"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="18"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="6">
@@ -7608,10 +7580,8 @@
       </c>
     </row>
     <row r="70" spans="2:34">
-      <c r="B70" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" s="17" t="s">
+      <c r="B70" s="12"/>
+      <c r="C70" s="14" t="s">
         <v>48</v>
       </c>
       <c r="D70" s="7" t="s">
@@ -7622,10 +7592,10 @@
         <v>0.5</v>
       </c>
       <c r="G70" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H70" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I70" s="9">
         <v>0</v>
@@ -7707,8 +7677,8 @@
       </c>
     </row>
     <row r="71" spans="2:34">
-      <c r="B71" s="16"/>
-      <c r="C71" s="19"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="6">
@@ -7717,11 +7687,11 @@
       </c>
       <c r="G71" s="6">
         <f t="shared" ref="G71:R71" si="41">AVERAGE(G70)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H71" s="6">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I71" s="6">
         <f t="shared" si="41"/>
@@ -7829,10 +7799,8 @@
       </c>
     </row>
     <row r="72" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B72" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="17" t="s">
+      <c r="B72" s="12"/>
+      <c r="C72" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D72" s="7" t="s">
@@ -7849,7 +7817,7 @@
         <v>0.75</v>
       </c>
       <c r="I72" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J72" s="9">
         <v>0</v>
@@ -7928,8 +7896,8 @@
       </c>
     </row>
     <row r="73" spans="2:34">
-      <c r="B73" s="15"/>
-      <c r="C73" s="18"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="15"/>
       <c r="D73" s="7" t="s">
         <v>47</v>
       </c>
@@ -7944,7 +7912,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J73" s="9">
         <v>0</v>
@@ -8023,8 +7991,8 @@
       </c>
     </row>
     <row r="74" spans="2:34">
-      <c r="B74" s="16"/>
-      <c r="C74" s="19"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="16"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="6">
@@ -8041,7 +8009,7 @@
       </c>
       <c r="I74" s="6">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="J74" s="6">
         <f t="shared" si="43"/>
@@ -8153,35 +8121,23 @@
       <c r="F76" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="B43:B50"/>
+  <mergeCells count="13">
+    <mergeCell ref="C6:C21"/>
+    <mergeCell ref="C27:C33"/>
+    <mergeCell ref="C34:C42"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="B6:B33"/>
+    <mergeCell ref="B34:B53"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C54:C67"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="B54:B74"/>
     <mergeCell ref="C43:C50"/>
-    <mergeCell ref="B51:B53"/>
     <mergeCell ref="C51:C53"/>
     <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C54:C67"/>
-    <mergeCell ref="B54:B67"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="C72:C74"/>
-    <mergeCell ref="C6:C21"/>
-    <mergeCell ref="B6:B21"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:C33"/>
-    <mergeCell ref="B34:B42"/>
-    <mergeCell ref="C34:C42"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="B72">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27:C27 E27:E28">
+  <conditionalFormatting sqref="C27 E27:E28">
     <cfRule type="cellIs" dxfId="9" priority="152" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -8191,7 +8147,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B43:D43 D43:D49">
+  <conditionalFormatting sqref="C43:D43 D43:D49">
     <cfRule type="cellIs" dxfId="7" priority="82" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -8206,7 +8162,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21 E22:E25 B54 B68">
+  <conditionalFormatting sqref="D21 E22:E25 B54">
     <cfRule type="cellIs" dxfId="4" priority="139" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -8273,7 +8229,21 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51 F54 F70 F55:AH66 F68:AH68">
+  <conditionalFormatting sqref="F45:F49 F43 F44:AH44">
+    <cfRule type="dataBar" priority="452">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FF147DFE-A319-4694-82C7-891FF6043D5B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51 F54 F55:AH66 F68:AH68 F70:H70">
     <cfRule type="dataBar" priority="444">
       <dataBar>
         <cfvo type="min"/>
@@ -8325,20 +8295,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{33F6A3E8-F39F-4486-821E-EFC74CA33142}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:F49 F43 F44:AH44">
-    <cfRule type="dataBar" priority="452">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FF147DFE-A319-4694-82C7-891FF6043D5B}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8413,7 +8369,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G51 G54 G70">
+  <conditionalFormatting sqref="G54 G51">
     <cfRule type="dataBar" priority="421">
       <dataBar>
         <cfvo type="min"/>
@@ -8539,7 +8495,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H51:AH51 H54:AH54 H70:AH70">
+  <conditionalFormatting sqref="H51:AH51 H54:AH54 I70:AH70">
     <cfRule type="dataBar" priority="465">
       <dataBar>
         <cfvo type="min"/>
@@ -8620,6 +8576,17 @@
           <xm:sqref>F38:F41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FF147DFE-A319-4694-82C7-891FF6043D5B}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F45:F49 F43 F44:AH44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{65D6EC0D-952A-420C-9BCF-6E4C561DF568}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
@@ -8628,7 +8595,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F51 F54 F70 F55:AH66 F68:AH68</xm:sqref>
+          <xm:sqref>F51 F54 F55:AH66 F68:AH68 F70:H70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9A642850-F1AC-4A64-AB4F-37A40B9CA441}">
@@ -8662,17 +8629,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>F22:G22 F24:G25 F23:AH23</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FF147DFE-A319-4694-82C7-891FF6043D5B}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F45:F49 F43 F44:AH44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1CEE6841-AF6F-4430-AD73-2BF608979F81}">
@@ -8738,7 +8694,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G51 G54 G70</xm:sqref>
+          <xm:sqref>G54 G51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{67C609FC-9661-4FF7-B05E-10F5DFEC8A7F}">
@@ -8837,7 +8793,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H51:AH51 H54:AH54 H70:AH70</xm:sqref>
+          <xm:sqref>H51:AH51 H54:AH54 I70:AH70</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5A887C91-57E6-4A6F-9712-7D026683BD38}">

</xml_diff>

<commit_message>
2025 02 07 // 17:00
</commit_message>
<xml_diff>
--- a/2팀(Pick+Course)보고양식.xlsx
+++ b/2팀(Pick+Course)보고양식.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gb_0900_jdy\git\workspace\pickcourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D36CD87-508A-48C9-963E-6FAAA713DB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE16226-6173-4762-B5C1-08B940ACA618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7995" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -311,6 +311,10 @@
     <t>신청자 상세 / 참여 승인 (모집자만)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>나의 후기 목록</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -475,7 +479,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -522,15 +526,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -551,10 +546,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -941,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AI75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1082,7 +1077,7 @@
       </c>
       <c r="L3" s="6">
         <f t="shared" si="0"/>
-        <v>0.58410714285714282</v>
+        <v>0.57624999999999993</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="0"/>
@@ -1274,7 +1269,7 @@
       <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1300,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M6" s="9">
         <v>0</v>
@@ -1371,7 +1366,7 @@
     </row>
     <row r="7" spans="2:34">
       <c r="B7" s="13"/>
-      <c r="C7" s="16"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="7" t="s">
         <v>47</v>
       </c>
@@ -1466,7 +1461,7 @@
     </row>
     <row r="8" spans="2:34">
       <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1561,7 +1556,7 @@
     </row>
     <row r="9" spans="2:34">
       <c r="B9" s="13"/>
-      <c r="C9" s="16"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="7" t="s">
         <v>7</v>
       </c>
@@ -1656,7 +1651,7 @@
     </row>
     <row r="10" spans="2:34">
       <c r="B10" s="13"/>
-      <c r="C10" s="16"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="7" t="s">
         <v>67</v>
       </c>
@@ -1751,7 +1746,7 @@
     </row>
     <row r="11" spans="2:34">
       <c r="B11" s="13"/>
-      <c r="C11" s="16"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
@@ -1846,7 +1841,7 @@
     </row>
     <row r="12" spans="2:34">
       <c r="B12" s="13"/>
-      <c r="C12" s="16"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1941,7 +1936,7 @@
     </row>
     <row r="13" spans="2:34">
       <c r="B13" s="13"/>
-      <c r="C13" s="16"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="7" t="s">
         <v>68</v>
       </c>
@@ -2036,7 +2031,7 @@
     </row>
     <row r="14" spans="2:34">
       <c r="B14" s="13"/>
-      <c r="C14" s="16"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
@@ -2131,7 +2126,7 @@
     </row>
     <row r="15" spans="2:34">
       <c r="B15" s="13"/>
-      <c r="C15" s="16"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
@@ -2226,7 +2221,7 @@
     </row>
     <row r="16" spans="2:34">
       <c r="B16" s="13"/>
-      <c r="C16" s="16"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2316,7 @@
     </row>
     <row r="17" spans="2:35">
       <c r="B17" s="13"/>
-      <c r="C17" s="16"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="7" t="s">
         <v>14</v>
       </c>
@@ -2416,9 +2411,9 @@
     </row>
     <row r="18" spans="2:35">
       <c r="B18" s="13"/>
-      <c r="C18" s="16"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="7" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="9">
@@ -2511,7 +2506,7 @@
     </row>
     <row r="19" spans="2:35">
       <c r="B19" s="13"/>
-      <c r="C19" s="16"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="7" t="s">
         <v>16</v>
       </c>
@@ -2606,7 +2601,7 @@
     </row>
     <row r="20" spans="2:35">
       <c r="B20" s="13"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="7" t="s">
         <v>20</v>
       </c>
@@ -2702,7 +2697,7 @@
     </row>
     <row r="21" spans="2:35">
       <c r="B21" s="13"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="7" t="s">
         <v>17</v>
       </c>
@@ -2797,7 +2792,7 @@
     </row>
     <row r="22" spans="2:35" ht="16.149999999999999" customHeight="1">
       <c r="B22" s="13"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="6">
@@ -2826,7 +2821,7 @@
       </c>
       <c r="L22" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="M22" s="6">
         <f t="shared" si="1"/>
@@ -2919,7 +2914,7 @@
     </row>
     <row r="23" spans="2:35">
       <c r="B23" s="13"/>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -3016,7 +3011,7 @@
     </row>
     <row r="24" spans="2:35">
       <c r="B24" s="13"/>
-      <c r="C24" s="19"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="7" t="s">
         <v>65</v>
       </c>
@@ -3111,7 +3106,7 @@
     </row>
     <row r="25" spans="2:35">
       <c r="B25" s="13"/>
-      <c r="C25" s="20"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="6">
@@ -3233,7 +3228,7 @@
     </row>
     <row r="26" spans="2:35">
       <c r="B26" s="13"/>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="21" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -3330,7 +3325,7 @@
     </row>
     <row r="27" spans="2:35">
       <c r="B27" s="13"/>
-      <c r="C27" s="25"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="7" t="s">
         <v>3</v>
       </c>
@@ -3425,7 +3420,7 @@
     </row>
     <row r="28" spans="2:35">
       <c r="B28" s="13"/>
-      <c r="C28" s="25"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="7" t="s">
         <v>63</v>
       </c>
@@ -3520,7 +3515,7 @@
     </row>
     <row r="29" spans="2:35">
       <c r="B29" s="13"/>
-      <c r="C29" s="25"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="7" t="s">
         <v>64</v>
       </c>
@@ -3615,7 +3610,7 @@
     </row>
     <row r="30" spans="2:35">
       <c r="B30" s="13"/>
-      <c r="C30" s="25"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="7" t="s">
         <v>19</v>
       </c>
@@ -3710,7 +3705,7 @@
     </row>
     <row r="31" spans="2:35">
       <c r="B31" s="14"/>
-      <c r="C31" s="26"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="6">
@@ -3831,10 +3826,10 @@
       </c>
     </row>
     <row r="32" spans="2:35">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -3930,8 +3925,8 @@
       </c>
     </row>
     <row r="33" spans="2:34">
-      <c r="B33" s="22"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="7" t="s">
         <v>49</v>
       </c>
@@ -4025,8 +4020,8 @@
       </c>
     </row>
     <row r="34" spans="2:34">
-      <c r="B34" s="22"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7" t="s">
         <v>54</v>
       </c>
@@ -4120,8 +4115,8 @@
       </c>
     </row>
     <row r="35" spans="2:34">
-      <c r="B35" s="22"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="7" t="s">
         <v>50</v>
       </c>
@@ -4215,8 +4210,8 @@
       </c>
     </row>
     <row r="36" spans="2:34">
-      <c r="B36" s="22"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="10" t="s">
         <v>51</v>
       </c>
@@ -4310,8 +4305,8 @@
       </c>
     </row>
     <row r="37" spans="2:34">
-      <c r="B37" s="22"/>
-      <c r="C37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="10" t="s">
         <v>52</v>
       </c>
@@ -4405,8 +4400,8 @@
       </c>
     </row>
     <row r="38" spans="2:34">
-      <c r="B38" s="22"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="10" t="s">
         <v>55</v>
       </c>
@@ -4430,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M38" s="9">
         <v>0</v>
@@ -4500,8 +4495,8 @@
       </c>
     </row>
     <row r="39" spans="2:34">
-      <c r="B39" s="22"/>
-      <c r="C39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="10" t="s">
         <v>56</v>
       </c>
@@ -4595,8 +4590,8 @@
       </c>
     </row>
     <row r="40" spans="2:34">
-      <c r="B40" s="22"/>
-      <c r="C40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="17"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="6">
@@ -4625,7 +4620,7 @@
       </c>
       <c r="L40" s="6">
         <f t="shared" si="5"/>
-        <v>0.71250000000000002</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="M40" s="6">
         <f t="shared" si="5"/>
@@ -4717,8 +4712,8 @@
       </c>
     </row>
     <row r="41" spans="2:34">
-      <c r="B41" s="22"/>
-      <c r="C41" s="18" t="s">
+      <c r="B41" s="19"/>
+      <c r="C41" s="15" t="s">
         <v>27</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -4814,8 +4809,8 @@
       </c>
     </row>
     <row r="42" spans="2:34">
-      <c r="B42" s="22"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="7" t="s">
         <v>60</v>
       </c>
@@ -4909,8 +4904,8 @@
       </c>
     </row>
     <row r="43" spans="2:34">
-      <c r="B43" s="22"/>
-      <c r="C43" s="19"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="7" t="s">
         <v>59</v>
       </c>
@@ -5004,8 +4999,8 @@
       </c>
     </row>
     <row r="44" spans="2:34">
-      <c r="B44" s="22"/>
-      <c r="C44" s="19"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="7" t="s">
         <v>48</v>
       </c>
@@ -5099,8 +5094,8 @@
       </c>
     </row>
     <row r="45" spans="2:34">
-      <c r="B45" s="22"/>
-      <c r="C45" s="19"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="10" t="s">
         <v>58</v>
       </c>
@@ -5194,8 +5189,8 @@
       </c>
     </row>
     <row r="46" spans="2:34">
-      <c r="B46" s="22"/>
-      <c r="C46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="10" t="s">
         <v>57</v>
       </c>
@@ -5289,8 +5284,8 @@
       </c>
     </row>
     <row r="47" spans="2:34">
-      <c r="B47" s="22"/>
-      <c r="C47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="7" t="s">
         <v>15</v>
       </c>
@@ -5314,7 +5309,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="9">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="M47" s="9">
         <v>0</v>
@@ -5384,8 +5379,8 @@
       </c>
     </row>
     <row r="48" spans="2:34">
-      <c r="B48" s="22"/>
-      <c r="C48" s="20"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="6">
@@ -5414,7 +5409,7 @@
       </c>
       <c r="L48" s="6">
         <f t="shared" si="6"/>
-        <v>0.98571428571428577</v>
+        <v>0.97142857142857153</v>
       </c>
       <c r="M48" s="6">
         <f t="shared" si="6"/>
@@ -5506,8 +5501,8 @@
       </c>
     </row>
     <row r="49" spans="2:34">
-      <c r="B49" s="22"/>
-      <c r="C49" s="19" t="s">
+      <c r="B49" s="19"/>
+      <c r="C49" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D49" s="7" t="s">
@@ -5603,8 +5598,8 @@
       </c>
     </row>
     <row r="50" spans="2:34">
-      <c r="B50" s="22"/>
-      <c r="C50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="7" t="s">
         <v>48</v>
       </c>
@@ -5698,8 +5693,8 @@
       </c>
     </row>
     <row r="51" spans="2:34">
-      <c r="B51" s="23"/>
-      <c r="C51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="17"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="6">
@@ -5820,10 +5815,10 @@
       </c>
     </row>
     <row r="52" spans="2:34">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="7" t="s">
@@ -5919,8 +5914,8 @@
       </c>
     </row>
     <row r="53" spans="2:34">
-      <c r="B53" s="22"/>
-      <c r="C53" s="19"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="7" t="s">
         <v>31</v>
       </c>
@@ -6014,8 +6009,8 @@
       </c>
     </row>
     <row r="54" spans="2:34">
-      <c r="B54" s="22"/>
-      <c r="C54" s="19"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="7" t="s">
         <v>32</v>
       </c>
@@ -6109,8 +6104,8 @@
       </c>
     </row>
     <row r="55" spans="2:34">
-      <c r="B55" s="22"/>
-      <c r="C55" s="19"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7" t="s">
         <v>33</v>
       </c>
@@ -6204,8 +6199,8 @@
       </c>
     </row>
     <row r="56" spans="2:34">
-      <c r="B56" s="22"/>
-      <c r="C56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="7" t="s">
         <v>21</v>
       </c>
@@ -6299,8 +6294,8 @@
       </c>
     </row>
     <row r="57" spans="2:34">
-      <c r="B57" s="22"/>
-      <c r="C57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="7" t="s">
         <v>22</v>
       </c>
@@ -6394,8 +6389,8 @@
       </c>
     </row>
     <row r="58" spans="2:34">
-      <c r="B58" s="22"/>
-      <c r="C58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="7" t="s">
         <v>34</v>
       </c>
@@ -6489,8 +6484,8 @@
       </c>
     </row>
     <row r="59" spans="2:34">
-      <c r="B59" s="22"/>
-      <c r="C59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="7" t="s">
         <v>35</v>
       </c>
@@ -6584,8 +6579,8 @@
       </c>
     </row>
     <row r="60" spans="2:34">
-      <c r="B60" s="22"/>
-      <c r="C60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="7" t="s">
         <v>7</v>
       </c>
@@ -6679,8 +6674,8 @@
       </c>
     </row>
     <row r="61" spans="2:34">
-      <c r="B61" s="22"/>
-      <c r="C61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="7" t="s">
         <v>8</v>
       </c>
@@ -6774,8 +6769,8 @@
       </c>
     </row>
     <row r="62" spans="2:34">
-      <c r="B62" s="22"/>
-      <c r="C62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7" t="s">
         <v>36</v>
       </c>
@@ -6799,7 +6794,7 @@
         <v>0.8</v>
       </c>
       <c r="L62" s="9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="M62" s="9">
         <v>0</v>
@@ -6869,8 +6864,8 @@
       </c>
     </row>
     <row r="63" spans="2:34">
-      <c r="B63" s="22"/>
-      <c r="C63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="7" t="s">
         <v>37</v>
       </c>
@@ -6964,8 +6959,8 @@
       </c>
     </row>
     <row r="64" spans="2:34">
-      <c r="B64" s="22"/>
-      <c r="C64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="7" t="s">
         <v>38</v>
       </c>
@@ -7059,8 +7054,8 @@
       </c>
     </row>
     <row r="65" spans="2:34">
-      <c r="B65" s="22"/>
-      <c r="C65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="7" t="s">
         <v>39</v>
       </c>
@@ -7154,8 +7149,8 @@
       </c>
     </row>
     <row r="66" spans="2:34">
-      <c r="B66" s="22"/>
-      <c r="C66" s="20"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="17"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="6">
@@ -7184,7 +7179,7 @@
       </c>
       <c r="L66" s="6">
         <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
+        <v>0.12857142857142859</v>
       </c>
       <c r="M66" s="6">
         <f t="shared" si="8"/>
@@ -7276,8 +7271,8 @@
       </c>
     </row>
     <row r="67" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B67" s="22"/>
-      <c r="C67" s="24" t="s">
+      <c r="B67" s="19"/>
+      <c r="C67" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D67" s="7" t="s">
@@ -7373,8 +7368,8 @@
       </c>
     </row>
     <row r="68" spans="2:34">
-      <c r="B68" s="22"/>
-      <c r="C68" s="26"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="6">
@@ -7495,8 +7490,8 @@
       </c>
     </row>
     <row r="69" spans="2:34">
-      <c r="B69" s="22"/>
-      <c r="C69" s="18" t="s">
+      <c r="B69" s="19"/>
+      <c r="C69" s="15" t="s">
         <v>44</v>
       </c>
       <c r="D69" s="7" t="s">
@@ -7592,8 +7587,8 @@
       </c>
     </row>
     <row r="70" spans="2:34">
-      <c r="B70" s="22"/>
-      <c r="C70" s="20"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="17"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="6">
@@ -7714,8 +7709,8 @@
       </c>
     </row>
     <row r="71" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B71" s="22"/>
-      <c r="C71" s="18" t="s">
+      <c r="B71" s="19"/>
+      <c r="C71" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D71" s="7" t="s">
@@ -7811,8 +7806,8 @@
       </c>
     </row>
     <row r="72" spans="2:34">
-      <c r="B72" s="22"/>
-      <c r="C72" s="19"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="16"/>
       <c r="D72" s="7" t="s">
         <v>43</v>
       </c>
@@ -7906,8 +7901,8 @@
       </c>
     </row>
     <row r="73" spans="2:34">
-      <c r="B73" s="23"/>
-      <c r="C73" s="20"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="17"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="6">
@@ -8036,18 +8031,19 @@
       <c r="F75" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="B52:B73"/>
-    <mergeCell ref="C41:C48"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="C67:C68"/>
+  <mergeCells count="12">
+    <mergeCell ref="C6:C22"/>
     <mergeCell ref="C32:C40"/>
     <mergeCell ref="B32:B51"/>
     <mergeCell ref="C26:C31"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C69:C70"/>
     <mergeCell ref="C52:C66"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="B52:B73"/>
+    <mergeCell ref="C41:C48"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="C67:C68"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C26 E26:E27">

</xml_diff>

<commit_message>
2025 02 17 // 13:23
</commit_message>
<xml_diff>
--- a/2팀(Pick+Course)보고양식.xlsx
+++ b/2팀(Pick+Course)보고양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gb_0900_jdy\git\workspace\pickcourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217544F7-3410-4EAF-8246-C3C26804E702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4670D10-A393-49D0-9102-B6D0771A45D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -303,6 +303,10 @@
     <t>코스 조회</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>코스 목록</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -467,7 +471,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -501,9 +505,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,24 +532,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -556,16 +539,6 @@
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -609,6 +582,16 @@
     <dxf>
       <font>
         <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
@@ -911,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AI69"/>
+  <dimension ref="B2:AH70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S55" sqref="S55"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -927,13 +910,14 @@
     <col min="6" max="6" width="9.875" style="8" hidden="1" customWidth="1"/>
     <col min="7" max="14" width="10.625" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="11.625" style="4" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.375" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="4"/>
+    <col min="16" max="16" width="11.5" style="4" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" style="4" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="11.375" style="4" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35">
+    <row r="2" spans="2:34">
       <c r="E2" s="2"/>
       <c r="F2" s="3">
         <v>45688</v>
@@ -1023,12 +1007,12 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="3" spans="2:35">
+    <row r="3" spans="2:34">
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:AH3" si="0">AVERAGE(F16,F19,F25,F35,F43,F46,F60,F62,F64,F67)</f>
+        <f t="shared" ref="F3:AH3" si="0">AVERAGE(F16,F19,F25,F35,F43,F46,F61,F63,F65,F68)</f>
         <v>0.06</v>
       </c>
       <c r="G3" s="6">
@@ -1069,31 +1053,31 @@
       </c>
       <c r="P3" s="6">
         <f t="shared" si="0"/>
-        <v>0.80384615384615399</v>
+        <v>0.79928571428571427</v>
       </c>
       <c r="Q3" s="6">
         <f t="shared" si="0"/>
-        <v>0.84792307692307689</v>
+        <v>0.84171428571428564</v>
       </c>
       <c r="R3" s="6">
         <f t="shared" si="0"/>
-        <v>0.95146153846153858</v>
+        <v>0.94585714285714284</v>
       </c>
       <c r="S3" s="6">
         <f t="shared" si="0"/>
-        <v>0.97399999999999987</v>
+        <v>0.96828571428571419</v>
       </c>
       <c r="T3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.97857142857142843</v>
       </c>
       <c r="U3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99285714285714288</v>
       </c>
       <c r="V3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" s="6">
         <f t="shared" si="0"/>
@@ -1144,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:35" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="2:34" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>0</v>
@@ -1241,11 +1225,11 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="6" spans="2:35">
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="2:34">
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="14" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1295,13 +1279,13 @@
         <v>1</v>
       </c>
       <c r="T6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="9">
         <v>0</v>
@@ -1340,9 +1324,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:35">
-      <c r="B7" s="18"/>
-      <c r="C7" s="22"/>
+    <row r="7" spans="2:34">
+      <c r="B7" s="17"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1390,13 +1374,13 @@
         <v>1</v>
       </c>
       <c r="T7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="9">
         <v>0</v>
@@ -1435,9 +1419,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:35">
-      <c r="B8" s="18"/>
-      <c r="C8" s="22"/>
+    <row r="8" spans="2:34">
+      <c r="B8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1485,13 +1469,13 @@
         <v>1</v>
       </c>
       <c r="T8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="9">
         <v>0</v>
@@ -1530,9 +1514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:35">
-      <c r="B9" s="18"/>
-      <c r="C9" s="22"/>
+    <row r="9" spans="2:34">
+      <c r="B9" s="17"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="7" t="s">
         <v>61</v>
       </c>
@@ -1580,13 +1564,13 @@
         <v>1</v>
       </c>
       <c r="T9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="9">
         <v>0</v>
@@ -1625,9 +1609,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:35">
-      <c r="B10" s="18"/>
-      <c r="C10" s="22"/>
+    <row r="10" spans="2:34">
+      <c r="B10" s="17"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
@@ -1675,13 +1659,13 @@
         <v>1</v>
       </c>
       <c r="T10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="9">
         <v>0</v>
@@ -1720,9 +1704,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:35">
-      <c r="B11" s="18"/>
-      <c r="C11" s="22"/>
+    <row r="11" spans="2:34">
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
@@ -1770,13 +1754,13 @@
         <v>1</v>
       </c>
       <c r="T11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="9">
         <v>0</v>
@@ -1815,9 +1799,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:35">
-      <c r="B12" s="18"/>
-      <c r="C12" s="22"/>
+    <row r="12" spans="2:34">
+      <c r="B12" s="17"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1865,13 +1849,13 @@
         <v>0.4</v>
       </c>
       <c r="T12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="9">
         <v>0</v>
@@ -1910,9 +1894,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:35">
-      <c r="B13" s="18"/>
-      <c r="C13" s="22"/>
+    <row r="13" spans="2:34">
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1960,13 +1944,13 @@
         <v>1</v>
       </c>
       <c r="T13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="9">
         <v>0</v>
@@ -2005,9 +1989,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:35">
-      <c r="B14" s="18"/>
-      <c r="C14" s="22"/>
+    <row r="14" spans="2:34">
+      <c r="B14" s="17"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="7" t="s">
         <v>14</v>
       </c>
@@ -2055,13 +2039,13 @@
         <v>1</v>
       </c>
       <c r="T14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="9">
         <v>0</v>
@@ -2099,11 +2083,10 @@
       <c r="AH14" s="9">
         <v>0</v>
       </c>
-      <c r="AI14" s="11"/>
     </row>
-    <row r="15" spans="2:35">
-      <c r="B15" s="18"/>
-      <c r="C15" s="22"/>
+    <row r="15" spans="2:34">
+      <c r="B15" s="17"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="7" t="s">
         <v>65</v>
       </c>
@@ -2151,13 +2134,13 @@
         <v>1</v>
       </c>
       <c r="T15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15" s="9">
         <v>0</v>
@@ -2196,131 +2179,131 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:35" ht="16.149999999999999" customHeight="1">
-      <c r="B16" s="18"/>
-      <c r="C16" s="23"/>
+    <row r="16" spans="2:34" ht="16.149999999999999" customHeight="1">
+      <c r="B16" s="17"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="6">
-        <f>AVERAGE(F6:F15)</f>
+        <f t="shared" ref="F16:AH16" si="1">AVERAGE(F6:F15)</f>
         <v>0</v>
       </c>
       <c r="G16" s="6">
-        <f>AVERAGE(G6:G15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H16" s="6">
-        <f>AVERAGE(H6:H15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I16" s="6">
-        <f>AVERAGE(I6:I15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J16" s="6">
-        <f>AVERAGE(J6:J15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K16" s="6">
-        <f>AVERAGE(K6:K15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L16" s="6">
-        <f>AVERAGE(L6:L15)</f>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="M16" s="6">
-        <f>AVERAGE(M6:M15)</f>
+        <f t="shared" si="1"/>
         <v>0.08</v>
       </c>
       <c r="N16" s="6">
-        <f>AVERAGE(N6:N15)</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="O16" s="6">
-        <f>AVERAGE(O6:O15)</f>
+        <f t="shared" si="1"/>
         <v>0.27999999999999997</v>
       </c>
       <c r="P16" s="6">
-        <f>AVERAGE(P6:P15)</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="Q16" s="6">
-        <f>AVERAGE(Q6:Q15)</f>
+        <f t="shared" si="1"/>
         <v>0.61</v>
       </c>
       <c r="R16" s="6">
-        <f>AVERAGE(R6:R15)</f>
+        <f t="shared" si="1"/>
         <v>0.73</v>
       </c>
       <c r="S16" s="6">
-        <f>AVERAGE(S6:S15)</f>
+        <f t="shared" si="1"/>
         <v>0.94000000000000006</v>
       </c>
       <c r="T16" s="6">
-        <f>AVERAGE(T6:T15)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="U16" s="6">
-        <f>AVERAGE(U6:U15)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="V16" s="6">
-        <f>AVERAGE(V6:V15)</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="W16" s="6">
-        <f>AVERAGE(W6:W15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="X16" s="6">
-        <f>AVERAGE(X6:X15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Y16" s="6">
-        <f>AVERAGE(Y6:Y15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Z16" s="6">
-        <f>AVERAGE(Z6:Z15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AA16" s="6">
-        <f>AVERAGE(AA6:AA15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AB16" s="6">
-        <f>AVERAGE(AB6:AB15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC16" s="6">
-        <f>AVERAGE(AC6:AC15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD16" s="6">
-        <f>AVERAGE(AD6:AD15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE16" s="6">
-        <f>AVERAGE(AE6:AE15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF16" s="6">
-        <f>AVERAGE(AF6:AF15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AG16" s="6">
-        <f>AVERAGE(AG6:AG15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AH16" s="6">
-        <f>AVERAGE(AH6:AH15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:34">
-      <c r="B17" s="18"/>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -2370,13 +2353,13 @@
         <v>1</v>
       </c>
       <c r="T17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="9">
         <v>0</v>
@@ -2416,8 +2399,8 @@
       </c>
     </row>
     <row r="18" spans="2:34">
-      <c r="B18" s="18"/>
-      <c r="C18" s="25"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="7" t="s">
         <v>59</v>
       </c>
@@ -2465,13 +2448,13 @@
         <v>1</v>
       </c>
       <c r="T18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="9">
         <v>0</v>
@@ -2511,40 +2494,40 @@
       </c>
     </row>
     <row r="19" spans="2:34">
-      <c r="B19" s="18"/>
-      <c r="C19" s="26"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6">
-        <f t="shared" ref="F19:AH19" si="1">AVERAGE(F17:F18)</f>
+        <f t="shared" ref="F19:AH19" si="2">AVERAGE(F17:F18)</f>
         <v>0</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
       <c r="K19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N19" s="6">
@@ -2552,11 +2535,11 @@
         <v>1</v>
       </c>
       <c r="O19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="P19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="Q19" s="6">
@@ -2564,77 +2547,77 @@
         <v>1</v>
       </c>
       <c r="R19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="S19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T19" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="U19" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="V19" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="W19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="X19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Y19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AB19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AC19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AD19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AE19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AF19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AG19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:34">
-      <c r="B20" s="18"/>
-      <c r="C20" s="15" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -2684,13 +2667,13 @@
         <v>1</v>
       </c>
       <c r="T20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="9">
         <v>0</v>
@@ -2730,8 +2713,8 @@
       </c>
     </row>
     <row r="21" spans="2:34">
-      <c r="B21" s="18"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
@@ -2779,13 +2762,13 @@
         <v>1</v>
       </c>
       <c r="T21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="9">
         <v>0</v>
@@ -2825,8 +2808,8 @@
       </c>
     </row>
     <row r="22" spans="2:34">
-      <c r="B22" s="18"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="7" t="s">
         <v>57</v>
       </c>
@@ -2874,13 +2857,13 @@
         <v>1</v>
       </c>
       <c r="T22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="9">
         <v>0</v>
@@ -2920,8 +2903,8 @@
       </c>
     </row>
     <row r="23" spans="2:34">
-      <c r="B23" s="18"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="7" t="s">
         <v>58</v>
       </c>
@@ -2969,13 +2952,13 @@
         <v>1</v>
       </c>
       <c r="T23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23" s="9">
         <v>0</v>
@@ -3015,8 +2998,8 @@
       </c>
     </row>
     <row r="24" spans="2:34">
-      <c r="B24" s="18"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="7" t="s">
         <v>13</v>
       </c>
@@ -3064,13 +3047,13 @@
         <v>1</v>
       </c>
       <c r="T24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="9">
         <v>0</v>
@@ -3110,40 +3093,40 @@
       </c>
     </row>
     <row r="25" spans="2:34">
-      <c r="B25" s="19"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="6">
-        <f t="shared" ref="F25:AH25" si="2">AVERAGE(F20:F24)</f>
+        <f t="shared" ref="F25:AH25" si="3">AVERAGE(F20:F24)</f>
         <v>0.1</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="H25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.27999999999999997</v>
       </c>
       <c r="J25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="N25" s="6">
@@ -3151,11 +3134,11 @@
         <v>1</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Q25" s="6">
@@ -3163,79 +3146,79 @@
         <v>1</v>
       </c>
       <c r="R25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U25" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="V25" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="W25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:34">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -3285,13 +3268,13 @@
         <v>1</v>
       </c>
       <c r="T26" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="9">
         <v>0</v>
@@ -3331,8 +3314,8 @@
       </c>
     </row>
     <row r="27" spans="2:34">
-      <c r="B27" s="18"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="7" t="s">
         <v>43</v>
       </c>
@@ -3380,13 +3363,13 @@
         <v>1</v>
       </c>
       <c r="T27" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U27" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V27" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="9">
         <v>0</v>
@@ -3426,8 +3409,8 @@
       </c>
     </row>
     <row r="28" spans="2:34">
-      <c r="B28" s="18"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="7" t="s">
         <v>48</v>
       </c>
@@ -3475,13 +3458,13 @@
         <v>1</v>
       </c>
       <c r="T28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W28" s="9">
         <v>0</v>
@@ -3521,8 +3504,8 @@
       </c>
     </row>
     <row r="29" spans="2:34">
-      <c r="B29" s="18"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="7" t="s">
         <v>44</v>
       </c>
@@ -3570,13 +3553,13 @@
         <v>1</v>
       </c>
       <c r="T29" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="9">
         <v>0</v>
@@ -3616,8 +3599,8 @@
       </c>
     </row>
     <row r="30" spans="2:34">
-      <c r="B30" s="18"/>
-      <c r="C30" s="13"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="10" t="s">
         <v>45</v>
       </c>
@@ -3665,13 +3648,13 @@
         <v>1</v>
       </c>
       <c r="T30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="9">
         <v>0</v>
@@ -3711,8 +3694,8 @@
       </c>
     </row>
     <row r="31" spans="2:34">
-      <c r="B31" s="18"/>
-      <c r="C31" s="13"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="10" t="s">
         <v>46</v>
       </c>
@@ -3760,13 +3743,13 @@
         <v>1</v>
       </c>
       <c r="T31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="9">
         <v>0</v>
@@ -3806,8 +3789,8 @@
       </c>
     </row>
     <row r="32" spans="2:34">
-      <c r="B32" s="18"/>
-      <c r="C32" s="13"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="10" t="s">
         <v>49</v>
       </c>
@@ -3855,13 +3838,13 @@
         <v>1</v>
       </c>
       <c r="T32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W32" s="9">
         <v>0</v>
@@ -3901,8 +3884,8 @@
       </c>
     </row>
     <row r="33" spans="2:34">
-      <c r="B33" s="18"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="10" t="s">
         <v>50</v>
       </c>
@@ -3950,13 +3933,13 @@
         <v>1</v>
       </c>
       <c r="T33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33" s="9">
         <v>0</v>
@@ -3996,8 +3979,8 @@
       </c>
     </row>
     <row r="34" spans="2:34">
-      <c r="B34" s="18"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="10" t="s">
         <v>63</v>
       </c>
@@ -4029,13 +4012,13 @@
         <v>1</v>
       </c>
       <c r="T34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W34" s="9">
         <v>0</v>
@@ -4075,40 +4058,40 @@
       </c>
     </row>
     <row r="35" spans="2:34">
-      <c r="B35" s="18"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="6">
-        <f t="shared" ref="F35:M35" si="3">AVERAGE(F26:F33)</f>
+        <f t="shared" ref="F35:M35" si="4">AVERAGE(F26:F33)</f>
         <v>0</v>
       </c>
       <c r="G35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
       <c r="I35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
       <c r="J35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
       <c r="K35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.625</v>
       </c>
       <c r="L35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="M35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.61250000000000004</v>
       </c>
       <c r="N35" s="6">
@@ -4116,11 +4099,11 @@
         <v>0.54444444444444451</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" ref="O35:AH35" si="4">AVERAGE(O26:O34)</f>
+        <f t="shared" ref="O35:AH35" si="5">AVERAGE(O26:O34)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="P35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="Q35" s="6">
@@ -4128,77 +4111,77 @@
         <v>1</v>
       </c>
       <c r="R35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="S35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="T35" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="U35" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="V35" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="W35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AH35" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="2:34">
-      <c r="B36" s="18"/>
-      <c r="C36" s="12" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -4248,13 +4231,13 @@
         <v>1</v>
       </c>
       <c r="T36" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V36" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W36" s="9">
         <v>0</v>
@@ -4294,8 +4277,8 @@
       </c>
     </row>
     <row r="37" spans="2:34">
-      <c r="B37" s="18"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="7" t="s">
         <v>54</v>
       </c>
@@ -4343,13 +4326,13 @@
         <v>1</v>
       </c>
       <c r="T37" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U37" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V37" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W37" s="9">
         <v>0</v>
@@ -4389,8 +4372,8 @@
       </c>
     </row>
     <row r="38" spans="2:34">
-      <c r="B38" s="18"/>
-      <c r="C38" s="13"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="7" t="s">
         <v>53</v>
       </c>
@@ -4438,13 +4421,13 @@
         <v>1</v>
       </c>
       <c r="T38" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V38" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38" s="9">
         <v>0</v>
@@ -4484,8 +4467,8 @@
       </c>
     </row>
     <row r="39" spans="2:34">
-      <c r="B39" s="18"/>
-      <c r="C39" s="13"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="7" t="s">
         <v>42</v>
       </c>
@@ -4533,13 +4516,13 @@
         <v>1</v>
       </c>
       <c r="T39" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V39" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W39" s="9">
         <v>0</v>
@@ -4579,8 +4562,8 @@
       </c>
     </row>
     <row r="40" spans="2:34">
-      <c r="B40" s="18"/>
-      <c r="C40" s="13"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="10" t="s">
         <v>52</v>
       </c>
@@ -4628,13 +4611,13 @@
         <v>1</v>
       </c>
       <c r="T40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W40" s="9">
         <v>0</v>
@@ -4674,8 +4657,8 @@
       </c>
     </row>
     <row r="41" spans="2:34">
-      <c r="B41" s="18"/>
-      <c r="C41" s="13"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="10" t="s">
         <v>51</v>
       </c>
@@ -4723,13 +4706,13 @@
         <v>1</v>
       </c>
       <c r="T41" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V41" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W41" s="9">
         <v>0</v>
@@ -4769,8 +4752,8 @@
       </c>
     </row>
     <row r="42" spans="2:34">
-      <c r="B42" s="18"/>
-      <c r="C42" s="13"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="7" t="s">
         <v>10</v>
       </c>
@@ -4818,13 +4801,13 @@
         <v>1</v>
       </c>
       <c r="T42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W42" s="9">
         <v>0</v>
@@ -4864,8 +4847,8 @@
       </c>
     </row>
     <row r="43" spans="2:34">
-      <c r="B43" s="18"/>
-      <c r="C43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="13"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="6">
@@ -4873,31 +4856,31 @@
         <v>0</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" ref="G43:AH43" si="5">AVERAGE(G36:G42)</f>
+        <f t="shared" ref="G43:AH43" si="6">AVERAGE(G36:G42)</f>
         <v>0</v>
       </c>
       <c r="H43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.84285714285714286</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="J43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.91428571428571437</v>
       </c>
       <c r="K43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.98285714285714287</v>
       </c>
       <c r="L43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97142857142857153</v>
       </c>
       <c r="M43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.97142857142857153</v>
       </c>
       <c r="N43" s="6">
@@ -4905,11 +4888,11 @@
         <v>0.97142857142857153</v>
       </c>
       <c r="O43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="P43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q43" s="6">
@@ -4917,77 +4900,77 @@
         <v>1</v>
       </c>
       <c r="R43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="S43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="T43" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="U43" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="V43" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="W43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AH43" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:34">
-      <c r="B44" s="18"/>
-      <c r="C44" s="13" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D44" s="7" t="s">
@@ -5037,13 +5020,13 @@
         <v>1</v>
       </c>
       <c r="T44" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U44" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V44" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44" s="9">
         <v>0</v>
@@ -5083,8 +5066,8 @@
       </c>
     </row>
     <row r="45" spans="2:34">
-      <c r="B45" s="18"/>
-      <c r="C45" s="13"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="7" t="s">
         <v>64</v>
       </c>
@@ -5132,13 +5115,13 @@
         <v>1</v>
       </c>
       <c r="T45" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V45" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W45" s="9">
         <v>0</v>
@@ -5178,8 +5161,8 @@
       </c>
     </row>
     <row r="46" spans="2:34">
-      <c r="B46" s="19"/>
-      <c r="C46" s="14"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="13"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="6">
@@ -5187,31 +5170,31 @@
         <v>0</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" ref="G46:AH46" si="6">AVERAGE(G44:G45)</f>
+        <f t="shared" ref="G46:AH46" si="7">AVERAGE(G44:G45)</f>
         <v>0</v>
       </c>
       <c r="H46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N46" s="6">
@@ -5219,91 +5202,91 @@
         <v>0</v>
       </c>
       <c r="O46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="Q46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="R46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="S46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="T46" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="U46" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="V46" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="W46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="X46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Y46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Z46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AC46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AF46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AG46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AH46" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:34">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D47" s="7" t="s">
@@ -5353,13 +5336,13 @@
         <v>1</v>
       </c>
       <c r="T47" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U47" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V47" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="9">
         <v>0</v>
@@ -5399,8 +5382,8 @@
       </c>
     </row>
     <row r="48" spans="2:34">
-      <c r="B48" s="18"/>
-      <c r="C48" s="13"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="12"/>
       <c r="D48" s="7" t="s">
         <v>25</v>
       </c>
@@ -5448,13 +5431,13 @@
         <v>1</v>
       </c>
       <c r="T48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="9">
         <v>0</v>
@@ -5494,8 +5477,8 @@
       </c>
     </row>
     <row r="49" spans="2:34">
-      <c r="B49" s="18"/>
-      <c r="C49" s="13"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="7" t="s">
         <v>26</v>
       </c>
@@ -5543,13 +5526,13 @@
         <v>1</v>
       </c>
       <c r="T49" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="9">
         <v>0</v>
@@ -5589,8 +5572,8 @@
       </c>
     </row>
     <row r="50" spans="2:34">
-      <c r="B50" s="18"/>
-      <c r="C50" s="13"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="12"/>
       <c r="D50" s="7" t="s">
         <v>27</v>
       </c>
@@ -5638,13 +5621,13 @@
         <v>1</v>
       </c>
       <c r="T50" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="9">
         <v>0</v>
@@ -5684,8 +5667,8 @@
       </c>
     </row>
     <row r="51" spans="2:34">
-      <c r="B51" s="18"/>
-      <c r="C51" s="13"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="12"/>
       <c r="D51" s="7" t="s">
         <v>15</v>
       </c>
@@ -5733,13 +5716,13 @@
         <v>1</v>
       </c>
       <c r="T51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W51" s="9">
         <v>0</v>
@@ -5779,8 +5762,8 @@
       </c>
     </row>
     <row r="52" spans="2:34">
-      <c r="B52" s="18"/>
-      <c r="C52" s="13"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="12"/>
       <c r="D52" s="7" t="s">
         <v>16</v>
       </c>
@@ -5828,13 +5811,13 @@
         <v>1</v>
       </c>
       <c r="T52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V52" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W52" s="9">
         <v>0</v>
@@ -5874,8 +5857,8 @@
       </c>
     </row>
     <row r="53" spans="2:34">
-      <c r="B53" s="18"/>
-      <c r="C53" s="13"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="12"/>
       <c r="D53" s="7" t="s">
         <v>28</v>
       </c>
@@ -5923,13 +5906,13 @@
         <v>1</v>
       </c>
       <c r="T53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V53" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W53" s="9">
         <v>0</v>
@@ -5969,8 +5952,8 @@
       </c>
     </row>
     <row r="54" spans="2:34">
-      <c r="B54" s="18"/>
-      <c r="C54" s="13"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="12"/>
       <c r="D54" s="7" t="s">
         <v>29</v>
       </c>
@@ -6018,13 +6001,13 @@
         <v>1</v>
       </c>
       <c r="T54" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U54" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V54" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W54" s="9">
         <v>0</v>
@@ -6064,42 +6047,22 @@
       </c>
     </row>
     <row r="55" spans="2:34">
-      <c r="B55" s="18"/>
-      <c r="C55" s="13"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="12"/>
       <c r="D55" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E55" s="7"/>
-      <c r="F55" s="9">
-        <v>0</v>
-      </c>
-      <c r="G55" s="9">
-        <v>0</v>
-      </c>
-      <c r="H55" s="9">
-        <v>0</v>
-      </c>
-      <c r="I55" s="9">
-        <v>0</v>
-      </c>
-      <c r="J55" s="9">
-        <v>0</v>
-      </c>
-      <c r="K55" s="9">
-        <v>0</v>
-      </c>
-      <c r="L55" s="9">
-        <v>0</v>
-      </c>
-      <c r="M55" s="9">
-        <v>0</v>
-      </c>
-      <c r="N55" s="9">
-        <v>0</v>
-      </c>
-      <c r="O55" s="9">
-        <v>0</v>
-      </c>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
       <c r="P55" s="9">
         <v>0</v>
       </c>
@@ -6116,10 +6079,10 @@
         <v>0</v>
       </c>
       <c r="U55" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W55" s="9">
         <v>0</v>
@@ -6159,10 +6122,10 @@
       </c>
     </row>
     <row r="56" spans="2:34">
-      <c r="B56" s="18"/>
-      <c r="C56" s="13"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="7" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="9">
@@ -6181,40 +6144,40 @@
         <v>0</v>
       </c>
       <c r="K56" s="9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="L56" s="9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M56" s="9">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="N56" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O56" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P56" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q56" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R56" s="9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="S56" s="9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="T56" s="9">
         <v>0</v>
       </c>
       <c r="U56" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V56" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W56" s="9">
         <v>0</v>
@@ -6254,10 +6217,10 @@
       </c>
     </row>
     <row r="57" spans="2:34">
-      <c r="B57" s="18"/>
-      <c r="C57" s="13"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="9">
@@ -6276,40 +6239,40 @@
         <v>0</v>
       </c>
       <c r="K57" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="L57" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M57" s="9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="N57" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O57" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P57" s="9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="Q57" s="9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="R57" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="S57" s="9">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="T57" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U57" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V57" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W57" s="9">
         <v>0</v>
@@ -6349,10 +6312,10 @@
       </c>
     </row>
     <row r="58" spans="2:34">
-      <c r="B58" s="18"/>
-      <c r="C58" s="13"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="9">
@@ -6386,25 +6349,25 @@
         <v>0</v>
       </c>
       <c r="P58" s="9">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="Q58" s="9">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="R58" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S58" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T58" s="9">
         <v>0</v>
       </c>
       <c r="U58" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V58" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W58" s="9">
         <v>0</v>
@@ -6444,10 +6407,10 @@
       </c>
     </row>
     <row r="59" spans="2:34">
-      <c r="B59" s="18"/>
-      <c r="C59" s="13"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="12"/>
       <c r="D59" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="9">
@@ -6493,13 +6456,13 @@
         <v>1</v>
       </c>
       <c r="T59" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U59" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V59" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59" s="9">
         <v>0</v>
@@ -6539,686 +6502,686 @@
       </c>
     </row>
     <row r="60" spans="2:34">
-      <c r="B60" s="18"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="7"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="E60" s="7"/>
-      <c r="F60" s="6">
-        <f t="shared" ref="F60:AH60" si="7">AVERAGE(F47:F59)</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="H60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="6">
-        <f t="shared" si="7"/>
+      <c r="F60" s="9">
+        <v>0</v>
+      </c>
+      <c r="G60" s="9">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9">
+        <v>0</v>
+      </c>
+      <c r="I60" s="9">
+        <v>0</v>
+      </c>
+      <c r="J60" s="9">
+        <v>0</v>
+      </c>
+      <c r="K60" s="9">
+        <v>0</v>
+      </c>
+      <c r="L60" s="9">
+        <v>0</v>
+      </c>
+      <c r="M60" s="9">
+        <v>0</v>
+      </c>
+      <c r="N60" s="9">
+        <v>0</v>
+      </c>
+      <c r="O60" s="9">
+        <v>0</v>
+      </c>
+      <c r="P60" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="9">
+        <v>1</v>
+      </c>
+      <c r="R60" s="9">
+        <v>1</v>
+      </c>
+      <c r="S60" s="9">
+        <v>1</v>
+      </c>
+      <c r="T60" s="9">
+        <v>1</v>
+      </c>
+      <c r="U60" s="9">
+        <v>1</v>
+      </c>
+      <c r="V60" s="9">
+        <v>1</v>
+      </c>
+      <c r="W60" s="9">
+        <v>0</v>
+      </c>
+      <c r="X60" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG60" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH60" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:34">
+      <c r="B61" s="17"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="6">
+        <f t="shared" ref="F61:AH61" si="8">AVERAGE(F47:F60)</f>
+        <v>0</v>
+      </c>
+      <c r="G61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="6">
+        <f t="shared" si="8"/>
         <v>3.4615384615384617E-2</v>
       </c>
-      <c r="K60" s="6">
-        <f t="shared" si="7"/>
+      <c r="K61" s="6">
+        <f t="shared" si="8"/>
         <v>0.13846153846153847</v>
       </c>
-      <c r="L60" s="6">
-        <f t="shared" si="7"/>
+      <c r="L61" s="6">
+        <f t="shared" si="8"/>
         <v>0.13846153846153847</v>
       </c>
-      <c r="M60" s="6">
-        <f t="shared" si="7"/>
+      <c r="M61" s="6">
+        <f t="shared" si="8"/>
         <v>0.15833333333333333</v>
       </c>
-      <c r="N60" s="6">
-        <f t="shared" si="7"/>
+      <c r="N61" s="6">
+        <f t="shared" si="8"/>
         <v>0.38461538461538464</v>
       </c>
-      <c r="O60" s="6">
-        <f t="shared" si="7"/>
+      <c r="O61" s="6">
+        <f t="shared" si="8"/>
         <v>0.46153846153846156</v>
       </c>
-      <c r="P60" s="6">
-        <f t="shared" si="7"/>
-        <v>0.63846153846153852</v>
-      </c>
-      <c r="Q60" s="6">
-        <f t="shared" si="7"/>
-        <v>0.86923076923076925</v>
-      </c>
-      <c r="R60" s="6">
-        <f t="shared" si="7"/>
-        <v>0.7846153846153846</v>
-      </c>
-      <c r="S60" s="6">
-        <f t="shared" si="7"/>
-        <v>0.8</v>
-      </c>
-      <c r="T60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="U60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="V60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AA60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AC60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AD60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AF60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AG60" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AH60" s="6">
-        <f t="shared" si="7"/>
+      <c r="P61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.59285714285714286</v>
+      </c>
+      <c r="Q61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.80714285714285716</v>
+      </c>
+      <c r="R61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.72857142857142854</v>
+      </c>
+      <c r="S61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="T61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.7857142857142857</v>
+      </c>
+      <c r="U61" s="6">
+        <f t="shared" si="8"/>
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="V61" s="6">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="W61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AD61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AE61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AF61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AG61" s="6">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AH61" s="6">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B61" s="18"/>
-      <c r="C61" s="15" t="s">
+    <row r="62" spans="2:34" ht="16.5" customHeight="1">
+      <c r="B62" s="17"/>
+      <c r="C62" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D62" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="9">
-        <v>0</v>
-      </c>
-      <c r="G61" s="9">
-        <v>0</v>
-      </c>
-      <c r="H61" s="9">
-        <v>0</v>
-      </c>
-      <c r="I61" s="9">
-        <v>0</v>
-      </c>
-      <c r="J61" s="9">
-        <v>0</v>
-      </c>
-      <c r="K61" s="9">
-        <v>0</v>
-      </c>
-      <c r="L61" s="9">
-        <v>0</v>
-      </c>
-      <c r="M61" s="9">
-        <v>0</v>
-      </c>
-      <c r="N61" s="9">
-        <v>0</v>
-      </c>
-      <c r="O61" s="9">
-        <v>0</v>
-      </c>
-      <c r="P61" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="9">
-        <v>0</v>
-      </c>
-      <c r="R61" s="9">
-        <v>1</v>
-      </c>
-      <c r="S61" s="9">
-        <v>1</v>
-      </c>
-      <c r="T61" s="9">
-        <v>0</v>
-      </c>
-      <c r="U61" s="9">
-        <v>0</v>
-      </c>
-      <c r="V61" s="9">
-        <v>0</v>
-      </c>
-      <c r="W61" s="9">
-        <v>0</v>
-      </c>
-      <c r="X61" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG61" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:34">
-      <c r="B62" s="18"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="7"/>
       <c r="E62" s="7"/>
-      <c r="F62" s="6">
-        <f>AVERAGE(F61)</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="6">
-        <f t="shared" ref="G62:AH62" si="8">AVERAGE(G61)</f>
-        <v>0</v>
-      </c>
-      <c r="H62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="M62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N62" s="6">
-        <f>AVERAGE(N61)</f>
-        <v>0</v>
-      </c>
-      <c r="O62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Q62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R62" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="S62" s="6">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="T62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="U62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="V62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="W62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="X62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG62" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH62" s="6">
-        <f t="shared" si="8"/>
+      <c r="F62" s="9">
+        <v>0</v>
+      </c>
+      <c r="G62" s="9">
+        <v>0</v>
+      </c>
+      <c r="H62" s="9">
+        <v>0</v>
+      </c>
+      <c r="I62" s="9">
+        <v>0</v>
+      </c>
+      <c r="J62" s="9">
+        <v>0</v>
+      </c>
+      <c r="K62" s="9">
+        <v>0</v>
+      </c>
+      <c r="L62" s="9">
+        <v>0</v>
+      </c>
+      <c r="M62" s="9">
+        <v>0</v>
+      </c>
+      <c r="N62" s="9">
+        <v>0</v>
+      </c>
+      <c r="O62" s="9">
+        <v>0</v>
+      </c>
+      <c r="P62" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="9">
+        <v>0</v>
+      </c>
+      <c r="R62" s="9">
+        <v>1</v>
+      </c>
+      <c r="S62" s="9">
+        <v>1</v>
+      </c>
+      <c r="T62" s="9">
+        <v>1</v>
+      </c>
+      <c r="U62" s="9">
+        <v>1</v>
+      </c>
+      <c r="V62" s="9">
+        <v>1</v>
+      </c>
+      <c r="W62" s="9">
+        <v>0</v>
+      </c>
+      <c r="X62" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:34">
-      <c r="B63" s="18"/>
-      <c r="C63" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G63" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="H63" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="I63" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="J63" s="9">
-        <v>1</v>
-      </c>
-      <c r="K63" s="9">
-        <v>1</v>
-      </c>
-      <c r="L63" s="9">
-        <v>1</v>
-      </c>
-      <c r="M63" s="9">
-        <v>1</v>
-      </c>
-      <c r="N63" s="9">
-        <v>1</v>
-      </c>
-      <c r="O63" s="9">
-        <v>1</v>
-      </c>
-      <c r="P63" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q63" s="9">
-        <v>1</v>
-      </c>
-      <c r="R63" s="9">
-        <v>1</v>
-      </c>
-      <c r="S63" s="9">
-        <v>1</v>
-      </c>
-      <c r="T63" s="9">
-        <v>0</v>
-      </c>
-      <c r="U63" s="9">
-        <v>0</v>
-      </c>
-      <c r="V63" s="9">
-        <v>0</v>
-      </c>
-      <c r="W63" s="9">
-        <v>0</v>
-      </c>
-      <c r="X63" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG63" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH63" s="9">
+      <c r="F63" s="6">
+        <f>AVERAGE(F62)</f>
+        <v>0</v>
+      </c>
+      <c r="G63" s="6">
+        <f t="shared" ref="G63:AH63" si="9">AVERAGE(G62)</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="6">
+        <f>AVERAGE(N62)</f>
+        <v>0</v>
+      </c>
+      <c r="O63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="R63" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="S63" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T63" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="U63" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="V63" s="6">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="W63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="X63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AG63" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AH63" s="6">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:34">
-      <c r="B64" s="18"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="7"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="6">
-        <f>AVERAGE(F63)</f>
+      <c r="F64" s="9">
         <v>0.5</v>
       </c>
-      <c r="G64" s="6">
-        <f t="shared" ref="G64:R64" si="9">AVERAGE(G63)</f>
+      <c r="G64" s="9">
         <v>0.5</v>
       </c>
-      <c r="H64" s="6">
-        <f t="shared" si="9"/>
+      <c r="H64" s="9">
         <v>0.5</v>
       </c>
-      <c r="I64" s="6">
-        <f t="shared" si="9"/>
+      <c r="I64" s="9">
         <v>0.5</v>
       </c>
-      <c r="J64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="K64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="L64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="M64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="N64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="O64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="P64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="Q64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="R64" s="6">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="S64" s="6">
-        <f t="shared" ref="S64:AH64" si="10">AVERAGE(S63)</f>
-        <v>1</v>
-      </c>
-      <c r="T64" s="6">
+      <c r="J64" s="9">
+        <v>1</v>
+      </c>
+      <c r="K64" s="9">
+        <v>1</v>
+      </c>
+      <c r="L64" s="9">
+        <v>1</v>
+      </c>
+      <c r="M64" s="9">
+        <v>1</v>
+      </c>
+      <c r="N64" s="9">
+        <v>1</v>
+      </c>
+      <c r="O64" s="9">
+        <v>1</v>
+      </c>
+      <c r="P64" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="9">
+        <v>1</v>
+      </c>
+      <c r="R64" s="9">
+        <v>1</v>
+      </c>
+      <c r="S64" s="9">
+        <v>1</v>
+      </c>
+      <c r="T64" s="9">
+        <v>1</v>
+      </c>
+      <c r="U64" s="9">
+        <v>1</v>
+      </c>
+      <c r="V64" s="9">
+        <v>1</v>
+      </c>
+      <c r="W64" s="9">
+        <v>0</v>
+      </c>
+      <c r="X64" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:34">
+      <c r="B65" s="17"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="6">
+        <f>AVERAGE(F64)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G65" s="6">
+        <f t="shared" ref="G65:R65" si="10">AVERAGE(G64)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="U64" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="I65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="V64" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="J65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="W64" s="6">
+        <v>1</v>
+      </c>
+      <c r="K65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="X64" s="6">
+        <v>1</v>
+      </c>
+      <c r="L65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Y64" s="6">
+        <v>1</v>
+      </c>
+      <c r="M65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Z64" s="6">
+        <v>1</v>
+      </c>
+      <c r="N65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AA64" s="6">
+        <v>1</v>
+      </c>
+      <c r="O65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB64" s="6">
+        <v>1</v>
+      </c>
+      <c r="P65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AC64" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AD64" s="6">
+        <v>1</v>
+      </c>
+      <c r="R65" s="6">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AE64" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AF64" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AG64" s="6">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AH64" s="6">
-        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="S65" s="6">
+        <f t="shared" ref="S65:AH65" si="11">AVERAGE(S64)</f>
+        <v>1</v>
+      </c>
+      <c r="T65" s="6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="U65" s="6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="V65" s="6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="W65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="X65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Y65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Z65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AA65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AB65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AC65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AD65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AE65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AG65" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH65" s="6">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B65" s="18"/>
-      <c r="C65" s="12" t="s">
+    <row r="66" spans="2:34" ht="16.5" customHeight="1">
+      <c r="B66" s="17"/>
+      <c r="C66" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D66" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="E65" s="7"/>
-      <c r="F65" s="9">
-        <v>0</v>
-      </c>
-      <c r="G65" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="H65" s="9">
-        <v>0.75</v>
-      </c>
-      <c r="I65" s="9">
-        <v>1</v>
-      </c>
-      <c r="J65" s="9">
-        <v>1</v>
-      </c>
-      <c r="K65" s="9">
-        <v>1</v>
-      </c>
-      <c r="L65" s="9">
-        <v>1</v>
-      </c>
-      <c r="M65" s="9">
-        <v>1</v>
-      </c>
-      <c r="N65" s="9">
-        <v>1</v>
-      </c>
-      <c r="O65" s="9">
-        <v>1</v>
-      </c>
-      <c r="P65" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="9">
-        <v>1</v>
-      </c>
-      <c r="R65" s="9">
-        <v>1</v>
-      </c>
-      <c r="S65" s="9">
-        <v>1</v>
-      </c>
-      <c r="T65" s="9">
-        <v>0</v>
-      </c>
-      <c r="U65" s="9">
-        <v>0</v>
-      </c>
-      <c r="V65" s="9">
-        <v>0</v>
-      </c>
-      <c r="W65" s="9">
-        <v>0</v>
-      </c>
-      <c r="X65" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG65" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH65" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:34">
-      <c r="B66" s="18"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="9">
         <v>0</v>
       </c>
       <c r="G66" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H66" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I66" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="J66" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="K66" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L66" s="9">
         <v>1</v>
@@ -7245,13 +7208,13 @@
         <v>1</v>
       </c>
       <c r="T66" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U66" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V66" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W66" s="9">
         <v>0</v>
@@ -7291,177 +7254,274 @@
       </c>
     </row>
     <row r="67" spans="2:34">
-      <c r="B67" s="19"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="7"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E67" s="7"/>
-      <c r="F67" s="6">
-        <f>AVERAGE(F65:F66)</f>
-        <v>0</v>
-      </c>
-      <c r="G67" s="6">
-        <f t="shared" ref="G67:R67" si="11">AVERAGE(G65:G66)</f>
-        <v>0.25</v>
-      </c>
-      <c r="H67" s="6">
-        <f t="shared" si="11"/>
-        <v>0.375</v>
-      </c>
-      <c r="I67" s="6">
-        <f t="shared" si="11"/>
-        <v>0.95</v>
-      </c>
-      <c r="J67" s="6">
-        <f t="shared" si="11"/>
-        <v>0.95</v>
-      </c>
-      <c r="K67" s="6">
-        <f t="shared" si="11"/>
-        <v>0.95</v>
-      </c>
-      <c r="L67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="M67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="N67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="O67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="P67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Q67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="R67" s="6">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="S67" s="6">
-        <f t="shared" ref="S67:AH67" si="12">AVERAGE(S65:S66)</f>
-        <v>1</v>
-      </c>
-      <c r="T67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="U67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="V67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="W67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="X67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Y67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="Z67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AA67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AB67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG67" s="6">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AH67" s="6">
-        <f t="shared" si="12"/>
+      <c r="F67" s="9">
+        <v>0</v>
+      </c>
+      <c r="G67" s="9">
+        <v>0</v>
+      </c>
+      <c r="H67" s="9">
+        <v>0</v>
+      </c>
+      <c r="I67" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="J67" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="K67" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="L67" s="9">
+        <v>1</v>
+      </c>
+      <c r="M67" s="9">
+        <v>1</v>
+      </c>
+      <c r="N67" s="9">
+        <v>1</v>
+      </c>
+      <c r="O67" s="9">
+        <v>1</v>
+      </c>
+      <c r="P67" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="9">
+        <v>1</v>
+      </c>
+      <c r="R67" s="9">
+        <v>1</v>
+      </c>
+      <c r="S67" s="9">
+        <v>1</v>
+      </c>
+      <c r="T67" s="9">
+        <v>1</v>
+      </c>
+      <c r="U67" s="9">
+        <v>1</v>
+      </c>
+      <c r="V67" s="9">
+        <v>1</v>
+      </c>
+      <c r="W67" s="9">
+        <v>0</v>
+      </c>
+      <c r="X67" s="9">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AE67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="9">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:34">
-      <c r="E68" s="8"/>
-      <c r="F68" s="4"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="6">
+        <f>AVERAGE(F66:F67)</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="6">
+        <f t="shared" ref="G68:R68" si="12">AVERAGE(G66:G67)</f>
+        <v>0.25</v>
+      </c>
+      <c r="H68" s="6">
+        <f t="shared" si="12"/>
+        <v>0.375</v>
+      </c>
+      <c r="I68" s="6">
+        <f t="shared" si="12"/>
+        <v>0.95</v>
+      </c>
+      <c r="J68" s="6">
+        <f t="shared" si="12"/>
+        <v>0.95</v>
+      </c>
+      <c r="K68" s="6">
+        <f t="shared" si="12"/>
+        <v>0.95</v>
+      </c>
+      <c r="L68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="M68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="N68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="O68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="P68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="Q68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="R68" s="6">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="S68" s="6">
+        <f t="shared" ref="S68:AH68" si="13">AVERAGE(S66:S67)</f>
+        <v>1</v>
+      </c>
+      <c r="T68" s="6">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="U68" s="6">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="V68" s="6">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="W68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="X68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Y68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Z68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AA68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AB68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AC68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AE68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AF68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AH68" s="6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="2:34">
       <c r="E69" s="8"/>
       <c r="F69" s="4"/>
     </row>
+    <row r="70" spans="2:34">
+      <c r="E70" s="8"/>
+      <c r="F70" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B47:B67"/>
-    <mergeCell ref="C47:C60"/>
+  <mergeCells count="13">
     <mergeCell ref="C26:C35"/>
     <mergeCell ref="B26:B46"/>
     <mergeCell ref="C20:C25"/>
     <mergeCell ref="B6:B25"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B47:B68"/>
+    <mergeCell ref="C6:C16"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C66:C68"/>
     <mergeCell ref="C36:C43"/>
     <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C47:C61"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="D6:D10 C36:D36 D36:D42 E6:E15">
-    <cfRule type="cellIs" dxfId="6" priority="115" operator="equal">
+  <conditionalFormatting sqref="C20 E20:E21">
+    <cfRule type="cellIs" dxfId="6" priority="185" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D34 D48:E60 D11:D15">
-    <cfRule type="cellIs" dxfId="5" priority="50" operator="equal">
+  <conditionalFormatting sqref="D6:D10 E6:E15 C36:D36 D36:D42">
+    <cfRule type="cellIs" dxfId="5" priority="115" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D15 D17:D34 D48:E61">
+    <cfRule type="cellIs" dxfId="4" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16 B47">
-    <cfRule type="cellIs" dxfId="4" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="172" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="cellIs" dxfId="3" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44:E44 D46:E46 C47:E47 C61:E61 D62:E67">
-    <cfRule type="cellIs" dxfId="2" priority="145" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20 E20:E21">
-    <cfRule type="cellIs" dxfId="1" priority="185" operator="equal">
+  <conditionalFormatting sqref="D44:E44 D46:E46 C47:E47 C62:E62 D63:E68">
+    <cfRule type="cellIs" dxfId="1" priority="145" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7596,7 +7656,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F65:F66">
+  <conditionalFormatting sqref="F66:F67">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -7610,7 +7670,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47:I59">
+  <conditionalFormatting sqref="F47:I60">
     <cfRule type="dataBar" priority="558">
       <dataBar>
         <cfvo type="min"/>
@@ -7624,7 +7684,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63:I63 F44">
+  <conditionalFormatting sqref="F64:I64 F44">
     <cfRule type="dataBar" priority="477">
       <dataBar>
         <cfvo type="min"/>
@@ -7634,6 +7694,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{65D6EC0D-952A-420C-9BCF-6E4C561DF568}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:AH15">
+    <cfRule type="dataBar" priority="651">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BE0275C9-A13C-4221-B9B7-203BFE7719CD}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -7652,7 +7726,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:AH61">
+  <conditionalFormatting sqref="F62:AH62">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
@@ -7778,7 +7852,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G65">
+  <conditionalFormatting sqref="G66">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -7792,7 +7866,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G66">
+  <conditionalFormatting sqref="G67">
     <cfRule type="dataBar" priority="462">
       <dataBar>
         <cfvo type="min"/>
@@ -7876,7 +7950,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H66">
+  <conditionalFormatting sqref="H67">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -7932,7 +8006,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65:K65">
+  <conditionalFormatting sqref="H66:K66">
     <cfRule type="dataBar" priority="488">
       <dataBar>
         <cfvo type="min"/>
@@ -7946,8 +8020,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:AH15 AI14">
-    <cfRule type="dataBar" priority="490">
+  <conditionalFormatting sqref="H6:AH15">
+    <cfRule type="dataBar" priority="652">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8044,7 +8118,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I66:K66">
+  <conditionalFormatting sqref="I67:K67">
     <cfRule type="dataBar" priority="502">
       <dataBar>
         <cfvo type="min"/>
@@ -8086,6 +8160,20 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J48:J49 J50:AH60">
+    <cfRule type="dataBar" priority="562">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{90455EE3-E7AD-4F59-8325-47922778E0F6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J26:K28">
     <cfRule type="dataBar" priority="28">
       <dataBar>
@@ -8114,7 +8202,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J63:K63 J47">
+  <conditionalFormatting sqref="J64:K64 J47">
     <cfRule type="dataBar" priority="498">
       <dataBar>
         <cfvo type="min"/>
@@ -8128,8 +8216,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J50:AH59 J48:J49">
-    <cfRule type="dataBar" priority="562">
+  <conditionalFormatting sqref="K36:O36 L40:O42 K38:O39 L37:O37 P36:AH42">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8137,21 +8225,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{90455EE3-E7AD-4F59-8325-47922778E0F6}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K32:AH32 K29:AH29 L26:AH28 L30:AH31">
-    <cfRule type="dataBar" priority="17">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5D6CA6F3-5CED-49CB-9FFA-6686FDCC177F}</x14:id>
+          <x14:id>{6C5573C3-41FA-4990-9C24-439EC153DA6C}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8198,7 +8272,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L63:AH63">
+  <conditionalFormatting sqref="L64:AH64">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
@@ -8212,7 +8286,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L65:AH66">
+  <conditionalFormatting sqref="L66:AH67">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -8226,8 +8300,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P36:AH42 K36:O36 L40:O42 K38:O39 L37:O37">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="W26:AH32 K32:V32 K29:V29 L26:V28 L30:V31">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8235,21 +8309,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6C5573C3-41FA-4990-9C24-439EC153DA6C}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:AH15">
-    <cfRule type="dataBar" priority="651">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BE0275C9-A13C-4221-B9B7-203BFE7719CD}</x14:id>
+          <x14:id>{5D6CA6F3-5CED-49CB-9FFA-6686FDCC177F}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8367,7 +8427,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F65:F66</xm:sqref>
+          <xm:sqref>F66:F67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6DB883C9-1F88-4735-AB90-2C226539E60C}">
@@ -8378,7 +8438,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F47:I59</xm:sqref>
+          <xm:sqref>F47:I60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{65D6EC0D-952A-420C-9BCF-6E4C561DF568}">
@@ -8389,7 +8449,18 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F63:I63 F44</xm:sqref>
+          <xm:sqref>F64:I64 F44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BE0275C9-A13C-4221-B9B7-203BFE7719CD}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F6:AH15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A0E20ECF-5663-478F-8E9F-449195CDAA9F}">
@@ -8411,7 +8482,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F61:AH61</xm:sqref>
+          <xm:sqref>F62:AH62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{57A8B765-FFA7-434C-9523-5857F06016E6}">
@@ -8510,7 +8581,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G65</xm:sqref>
+          <xm:sqref>G66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6182F17D-C40E-44F1-A805-62C9A04B4BC8}">
@@ -8521,7 +8592,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G66</xm:sqref>
+          <xm:sqref>G67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3AE68020-C365-4ABF-939B-EF0068109146}">
@@ -8587,7 +8658,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H66</xm:sqref>
+          <xm:sqref>H67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1303D586-8258-463C-8ABD-037215FABF40}">
@@ -8631,7 +8702,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H65:K65</xm:sqref>
+          <xm:sqref>H66:K66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BC994E96-D1FB-4FF1-98B0-81DBE99950DE}">
@@ -8642,7 +8713,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H6:AH15 AI14</xm:sqref>
+          <xm:sqref>H6:AH15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5A887C91-57E6-4A6F-9712-7D026683BD38}">
@@ -8719,7 +8790,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I66:K66</xm:sqref>
+          <xm:sqref>I67:K67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{196E49F1-0D91-4E01-BC7E-8AB3EB3E8E66}">
@@ -8742,6 +8813,17 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>J39:J42 K40:K42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{90455EE3-E7AD-4F59-8325-47922778E0F6}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J48:J49 J50:AH60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DBDB9E12-FBD7-4ED7-8AF2-CC272D920CAD}">
@@ -8774,10 +8856,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J63:K63 J47</xm:sqref>
+          <xm:sqref>J64:K64 J47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{90455EE3-E7AD-4F59-8325-47922778E0F6}">
+          <x14:cfRule type="dataBar" id="{6C5573C3-41FA-4990-9C24-439EC153DA6C}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8785,18 +8867,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J50:AH59 J48:J49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5D6CA6F3-5CED-49CB-9FFA-6686FDCC177F}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>K32:AH32 K29:AH29 L26:AH28 L30:AH31</xm:sqref>
+          <xm:sqref>K36:O36 L40:O42 K38:O39 L37:O37 P36:AH42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{79A6E942-BB28-4C5C-B051-63D2113FB72F}">
@@ -8840,7 +8911,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L63:AH63</xm:sqref>
+          <xm:sqref>L64:AH64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B769FDA4-52DD-48E5-B5B4-67E966D84479}">
@@ -8851,10 +8922,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L65:AH66</xm:sqref>
+          <xm:sqref>L66:AH67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6C5573C3-41FA-4990-9C24-439EC153DA6C}">
+          <x14:cfRule type="dataBar" id="{5D6CA6F3-5CED-49CB-9FFA-6686FDCC177F}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -8862,18 +8933,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>P36:AH42 K36:O36 L40:O42 K38:O39 L37:O37</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BE0275C9-A13C-4221-B9B7-203BFE7719CD}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F6:AH15</xm:sqref>
+          <xm:sqref>W26:AH32 K32:V32 K29:V29 L26:V28 L30:V31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
2025 02 17 // 16:51
</commit_message>
<xml_diff>
--- a/2팀(Pick+Course)보고양식.xlsx
+++ b/2팀(Pick+Course)보고양식.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gb_0900_jdy\git\workspace\pickcourse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4670D10-A393-49D0-9102-B6D0771A45D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D78182-39AA-4F8D-93D4-A5D82A16907B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,12 +514,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,7 +523,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -894,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AH70"/>
+  <dimension ref="B2:V70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C19"/>
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -917,7 +917,7 @@
     <col min="20" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:34">
+    <row r="2" spans="2:22">
       <c r="E2" s="2"/>
       <c r="F2" s="3">
         <v>45688</v>
@@ -970,49 +970,13 @@
       <c r="V2" s="3">
         <v>45704</v>
       </c>
-      <c r="W2" s="3">
-        <v>45705</v>
-      </c>
-      <c r="X2" s="3">
-        <v>45706</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>45707</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>45708</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>45709</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>45710</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>45711</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>45712</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>45713</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>45714</v>
-      </c>
-      <c r="AG2" s="3">
-        <v>45715</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="3" spans="2:34">
+    </row>
+    <row r="3" spans="2:22">
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="6">
-        <f t="shared" ref="F3:AH3" si="0">AVERAGE(F16,F19,F25,F35,F43,F46,F61,F63,F65,F68)</f>
+        <f t="shared" ref="F3:V3" si="0">AVERAGE(F16,F19,F25,F35,F43,F46,F61,F63,F65,F68)</f>
         <v>0.06</v>
       </c>
       <c r="G3" s="6">
@@ -1079,56 +1043,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH3" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:34" ht="20.100000000000001" customHeight="1">
+    </row>
+    <row r="5" spans="2:22" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
         <v>0</v>
@@ -1188,48 +1104,12 @@
       <c r="V5" s="3">
         <v>45704</v>
       </c>
-      <c r="W5" s="3">
-        <v>45705</v>
-      </c>
-      <c r="X5" s="3">
-        <v>45706</v>
-      </c>
-      <c r="Y5" s="3">
-        <v>45707</v>
-      </c>
-      <c r="Z5" s="3">
-        <v>45708</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>45709</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>45710</v>
-      </c>
-      <c r="AC5" s="3">
-        <v>45711</v>
-      </c>
-      <c r="AD5" s="3">
-        <v>45712</v>
-      </c>
-      <c r="AE5" s="3">
-        <v>45713</v>
-      </c>
-      <c r="AF5" s="3">
-        <v>45714</v>
-      </c>
-      <c r="AG5" s="3">
-        <v>45715</v>
-      </c>
-      <c r="AH5" s="3">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="6" spans="2:34">
-      <c r="B6" s="16" t="s">
+    </row>
+    <row r="6" spans="2:22">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1287,46 +1167,10 @@
       <c r="V6" s="9">
         <v>1</v>
       </c>
-      <c r="W6" s="9">
-        <v>0</v>
-      </c>
-      <c r="X6" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:34">
-      <c r="B7" s="17"/>
-      <c r="C7" s="19"/>
+    </row>
+    <row r="7" spans="2:22">
+      <c r="B7" s="15"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1382,46 +1226,10 @@
       <c r="V7" s="9">
         <v>1</v>
       </c>
-      <c r="W7" s="9">
-        <v>0</v>
-      </c>
-      <c r="X7" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:34">
-      <c r="B8" s="17"/>
-      <c r="C8" s="19"/>
+    </row>
+    <row r="8" spans="2:22">
+      <c r="B8" s="15"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="7" t="s">
         <v>6</v>
       </c>
@@ -1477,46 +1285,10 @@
       <c r="V8" s="9">
         <v>1</v>
       </c>
-      <c r="W8" s="9">
-        <v>0</v>
-      </c>
-      <c r="X8" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:34">
-      <c r="B9" s="17"/>
-      <c r="C9" s="19"/>
+    </row>
+    <row r="9" spans="2:22">
+      <c r="B9" s="15"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="7" t="s">
         <v>61</v>
       </c>
@@ -1572,46 +1344,10 @@
       <c r="V9" s="9">
         <v>1</v>
       </c>
-      <c r="W9" s="9">
-        <v>0</v>
-      </c>
-      <c r="X9" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:34">
-      <c r="B10" s="17"/>
-      <c r="C10" s="19"/>
+    </row>
+    <row r="10" spans="2:22">
+      <c r="B10" s="15"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="7" t="s">
         <v>7</v>
       </c>
@@ -1667,46 +1403,10 @@
       <c r="V10" s="9">
         <v>1</v>
       </c>
-      <c r="W10" s="9">
-        <v>0</v>
-      </c>
-      <c r="X10" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:34">
-      <c r="B11" s="17"/>
-      <c r="C11" s="19"/>
+    </row>
+    <row r="11" spans="2:22">
+      <c r="B11" s="15"/>
+      <c r="C11" s="18"/>
       <c r="D11" s="7" t="s">
         <v>8</v>
       </c>
@@ -1762,46 +1462,10 @@
       <c r="V11" s="9">
         <v>1</v>
       </c>
-      <c r="W11" s="9">
-        <v>0</v>
-      </c>
-      <c r="X11" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:34">
-      <c r="B12" s="17"/>
-      <c r="C12" s="19"/>
+    </row>
+    <row r="12" spans="2:22">
+      <c r="B12" s="15"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="7" t="s">
         <v>9</v>
       </c>
@@ -1857,46 +1521,10 @@
       <c r="V12" s="9">
         <v>1</v>
       </c>
-      <c r="W12" s="9">
-        <v>0</v>
-      </c>
-      <c r="X12" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:34">
-      <c r="B13" s="17"/>
-      <c r="C13" s="19"/>
+    </row>
+    <row r="13" spans="2:22">
+      <c r="B13" s="15"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1952,46 +1580,10 @@
       <c r="V13" s="9">
         <v>1</v>
       </c>
-      <c r="W13" s="9">
-        <v>0</v>
-      </c>
-      <c r="X13" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:34">
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
+    </row>
+    <row r="14" spans="2:22">
+      <c r="B14" s="15"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="7" t="s">
         <v>14</v>
       </c>
@@ -2047,46 +1639,10 @@
       <c r="V14" s="9">
         <v>1</v>
       </c>
-      <c r="W14" s="9">
-        <v>0</v>
-      </c>
-      <c r="X14" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:34">
-      <c r="B15" s="17"/>
-      <c r="C15" s="19"/>
+    </row>
+    <row r="15" spans="2:22">
+      <c r="B15" s="15"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="7" t="s">
         <v>65</v>
       </c>
@@ -2142,50 +1698,14 @@
       <c r="V15" s="9">
         <v>1</v>
       </c>
-      <c r="W15" s="9">
-        <v>0</v>
-      </c>
-      <c r="X15" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:34" ht="16.149999999999999" customHeight="1">
-      <c r="B16" s="17"/>
-      <c r="C16" s="15"/>
+    </row>
+    <row r="16" spans="2:22" ht="16.149999999999999" customHeight="1">
+      <c r="B16" s="15"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="6">
-        <f t="shared" ref="F16:AH16" si="1">AVERAGE(F6:F15)</f>
+        <f t="shared" ref="F16:V16" si="1">AVERAGE(F6:F15)</f>
         <v>0</v>
       </c>
       <c r="G16" s="6">
@@ -2252,57 +1772,9 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="W16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="X16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AA16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AB16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AC16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AD16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AE16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AG16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AH16" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:34">
-      <c r="B17" s="17"/>
+    </row>
+    <row r="17" spans="2:22">
+      <c r="B17" s="15"/>
       <c r="C17" s="11" t="s">
         <v>18</v>
       </c>
@@ -2361,45 +1833,9 @@
       <c r="V17" s="9">
         <v>1</v>
       </c>
-      <c r="W17" s="9">
-        <v>0</v>
-      </c>
-      <c r="X17" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:34">
-      <c r="B18" s="17"/>
+    </row>
+    <row r="18" spans="2:22">
+      <c r="B18" s="15"/>
       <c r="C18" s="12"/>
       <c r="D18" s="7" t="s">
         <v>59</v>
@@ -2456,50 +1892,14 @@
       <c r="V18" s="9">
         <v>1</v>
       </c>
-      <c r="W18" s="9">
-        <v>0</v>
-      </c>
-      <c r="X18" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:34">
-      <c r="B19" s="17"/>
+    </row>
+    <row r="19" spans="2:22">
+      <c r="B19" s="15"/>
       <c r="C19" s="13"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6">
-        <f t="shared" ref="F19:AH19" si="2">AVERAGE(F17:F18)</f>
+        <f t="shared" ref="F19:V19" si="2">AVERAGE(F17:F18)</f>
         <v>0</v>
       </c>
       <c r="G19" s="6">
@@ -2566,58 +1966,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="W19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AB19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AC19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AD19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AE19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AF19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AG19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AH19" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:34">
-      <c r="B20" s="17"/>
-      <c r="C20" s="14" t="s">
+    </row>
+    <row r="20" spans="2:22">
+      <c r="B20" s="15"/>
+      <c r="C20" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="7" t="s">
@@ -2675,46 +2027,10 @@
       <c r="V20" s="9">
         <v>1</v>
       </c>
-      <c r="W20" s="9">
-        <v>0</v>
-      </c>
-      <c r="X20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:34">
-      <c r="B21" s="17"/>
-      <c r="C21" s="19"/>
+    </row>
+    <row r="21" spans="2:22">
+      <c r="B21" s="15"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
@@ -2770,46 +2086,10 @@
       <c r="V21" s="9">
         <v>1</v>
       </c>
-      <c r="W21" s="9">
-        <v>0</v>
-      </c>
-      <c r="X21" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:34">
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
+    </row>
+    <row r="22" spans="2:22">
+      <c r="B22" s="15"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="7" t="s">
         <v>57</v>
       </c>
@@ -2865,46 +2145,10 @@
       <c r="V22" s="9">
         <v>1</v>
       </c>
-      <c r="W22" s="9">
-        <v>0</v>
-      </c>
-      <c r="X22" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH22" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:34">
-      <c r="B23" s="17"/>
-      <c r="C23" s="19"/>
+    </row>
+    <row r="23" spans="2:22">
+      <c r="B23" s="15"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="7" t="s">
         <v>58</v>
       </c>
@@ -2960,46 +2204,10 @@
       <c r="V23" s="9">
         <v>1</v>
       </c>
-      <c r="W23" s="9">
-        <v>0</v>
-      </c>
-      <c r="X23" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:34">
-      <c r="B24" s="17"/>
-      <c r="C24" s="19"/>
+    </row>
+    <row r="24" spans="2:22">
+      <c r="B24" s="15"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="7" t="s">
         <v>13</v>
       </c>
@@ -3055,50 +2263,14 @@
       <c r="V24" s="9">
         <v>1</v>
       </c>
-      <c r="W24" s="9">
-        <v>0</v>
-      </c>
-      <c r="X24" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:34">
-      <c r="B25" s="18"/>
-      <c r="C25" s="15"/>
+    </row>
+    <row r="25" spans="2:22">
+      <c r="B25" s="16"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="6">
-        <f t="shared" ref="F25:AH25" si="3">AVERAGE(F20:F24)</f>
+        <f t="shared" ref="F25:V25" si="3">AVERAGE(F20:F24)</f>
         <v>0.1</v>
       </c>
       <c r="G25" s="6">
@@ -3165,57 +2337,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="W25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="X25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Y25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="Z25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AE25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AF25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:34">
-      <c r="B26" s="16" t="s">
+    </row>
+    <row r="26" spans="2:22">
+      <c r="B26" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -3276,45 +2400,9 @@
       <c r="V26" s="9">
         <v>1</v>
       </c>
-      <c r="W26" s="9">
-        <v>0</v>
-      </c>
-      <c r="X26" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH26" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:34">
-      <c r="B27" s="17"/>
+    </row>
+    <row r="27" spans="2:22">
+      <c r="B27" s="15"/>
       <c r="C27" s="12"/>
       <c r="D27" s="7" t="s">
         <v>43</v>
@@ -3371,45 +2459,9 @@
       <c r="V27" s="9">
         <v>1</v>
       </c>
-      <c r="W27" s="9">
-        <v>0</v>
-      </c>
-      <c r="X27" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG27" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:34">
-      <c r="B28" s="17"/>
+    </row>
+    <row r="28" spans="2:22">
+      <c r="B28" s="15"/>
       <c r="C28" s="12"/>
       <c r="D28" s="7" t="s">
         <v>48</v>
@@ -3466,45 +2518,9 @@
       <c r="V28" s="9">
         <v>1</v>
       </c>
-      <c r="W28" s="9">
-        <v>0</v>
-      </c>
-      <c r="X28" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:34">
-      <c r="B29" s="17"/>
+    </row>
+    <row r="29" spans="2:22">
+      <c r="B29" s="15"/>
       <c r="C29" s="12"/>
       <c r="D29" s="7" t="s">
         <v>44</v>
@@ -3561,45 +2577,9 @@
       <c r="V29" s="9">
         <v>1</v>
       </c>
-      <c r="W29" s="9">
-        <v>0</v>
-      </c>
-      <c r="X29" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:34">
-      <c r="B30" s="17"/>
+    </row>
+    <row r="30" spans="2:22">
+      <c r="B30" s="15"/>
       <c r="C30" s="12"/>
       <c r="D30" s="10" t="s">
         <v>45</v>
@@ -3656,45 +2636,9 @@
       <c r="V30" s="9">
         <v>1</v>
       </c>
-      <c r="W30" s="9">
-        <v>0</v>
-      </c>
-      <c r="X30" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG30" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH30" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:34">
-      <c r="B31" s="17"/>
+    </row>
+    <row r="31" spans="2:22">
+      <c r="B31" s="15"/>
       <c r="C31" s="12"/>
       <c r="D31" s="10" t="s">
         <v>46</v>
@@ -3751,45 +2695,9 @@
       <c r="V31" s="9">
         <v>1</v>
       </c>
-      <c r="W31" s="9">
-        <v>0</v>
-      </c>
-      <c r="X31" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG31" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH31" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:34">
-      <c r="B32" s="17"/>
+    </row>
+    <row r="32" spans="2:22">
+      <c r="B32" s="15"/>
       <c r="C32" s="12"/>
       <c r="D32" s="10" t="s">
         <v>49</v>
@@ -3846,45 +2754,9 @@
       <c r="V32" s="9">
         <v>1</v>
       </c>
-      <c r="W32" s="9">
-        <v>0</v>
-      </c>
-      <c r="X32" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH32" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:34">
-      <c r="B33" s="17"/>
+    </row>
+    <row r="33" spans="2:22">
+      <c r="B33" s="15"/>
       <c r="C33" s="12"/>
       <c r="D33" s="10" t="s">
         <v>50</v>
@@ -3941,45 +2813,9 @@
       <c r="V33" s="9">
         <v>1</v>
       </c>
-      <c r="W33" s="9">
-        <v>0</v>
-      </c>
-      <c r="X33" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH33" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:34">
-      <c r="B34" s="17"/>
+    </row>
+    <row r="34" spans="2:22">
+      <c r="B34" s="15"/>
       <c r="C34" s="12"/>
       <c r="D34" s="10" t="s">
         <v>63</v>
@@ -4020,45 +2856,9 @@
       <c r="V34" s="9">
         <v>1</v>
       </c>
-      <c r="W34" s="9">
-        <v>0</v>
-      </c>
-      <c r="X34" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH34" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:34">
-      <c r="B35" s="17"/>
+    </row>
+    <row r="35" spans="2:22">
+      <c r="B35" s="15"/>
       <c r="C35" s="13"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -4099,7 +2899,7 @@
         <v>0.54444444444444451</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" ref="O35:AH35" si="5">AVERAGE(O26:O34)</f>
+        <f t="shared" ref="O35:V35" si="5">AVERAGE(O26:O34)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="P35" s="6">
@@ -4130,57 +2930,9 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="W35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AA35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AB35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AC35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AD35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AE35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AF35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AG35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AH35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:34">
-      <c r="B36" s="17"/>
+    </row>
+    <row r="36" spans="2:22">
+      <c r="B36" s="15"/>
       <c r="C36" s="11" t="s">
         <v>21</v>
       </c>
@@ -4239,45 +2991,9 @@
       <c r="V36" s="9">
         <v>1</v>
       </c>
-      <c r="W36" s="9">
-        <v>0</v>
-      </c>
-      <c r="X36" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:34">
-      <c r="B37" s="17"/>
+    </row>
+    <row r="37" spans="2:22">
+      <c r="B37" s="15"/>
       <c r="C37" s="12"/>
       <c r="D37" s="7" t="s">
         <v>54</v>
@@ -4334,45 +3050,9 @@
       <c r="V37" s="9">
         <v>1</v>
       </c>
-      <c r="W37" s="9">
-        <v>0</v>
-      </c>
-      <c r="X37" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH37" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:34">
-      <c r="B38" s="17"/>
+    </row>
+    <row r="38" spans="2:22">
+      <c r="B38" s="15"/>
       <c r="C38" s="12"/>
       <c r="D38" s="7" t="s">
         <v>53</v>
@@ -4429,45 +3109,9 @@
       <c r="V38" s="9">
         <v>1</v>
       </c>
-      <c r="W38" s="9">
-        <v>0</v>
-      </c>
-      <c r="X38" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:34">
-      <c r="B39" s="17"/>
+    </row>
+    <row r="39" spans="2:22">
+      <c r="B39" s="15"/>
       <c r="C39" s="12"/>
       <c r="D39" s="7" t="s">
         <v>42</v>
@@ -4524,45 +3168,9 @@
       <c r="V39" s="9">
         <v>1</v>
       </c>
-      <c r="W39" s="9">
-        <v>0</v>
-      </c>
-      <c r="X39" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:34">
-      <c r="B40" s="17"/>
+    </row>
+    <row r="40" spans="2:22">
+      <c r="B40" s="15"/>
       <c r="C40" s="12"/>
       <c r="D40" s="10" t="s">
         <v>52</v>
@@ -4619,45 +3227,9 @@
       <c r="V40" s="9">
         <v>1</v>
       </c>
-      <c r="W40" s="9">
-        <v>0</v>
-      </c>
-      <c r="X40" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:34">
-      <c r="B41" s="17"/>
+    </row>
+    <row r="41" spans="2:22">
+      <c r="B41" s="15"/>
       <c r="C41" s="12"/>
       <c r="D41" s="10" t="s">
         <v>51</v>
@@ -4714,45 +3286,9 @@
       <c r="V41" s="9">
         <v>1</v>
       </c>
-      <c r="W41" s="9">
-        <v>0</v>
-      </c>
-      <c r="X41" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG41" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH41" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:34">
-      <c r="B42" s="17"/>
+    </row>
+    <row r="42" spans="2:22">
+      <c r="B42" s="15"/>
       <c r="C42" s="12"/>
       <c r="D42" s="7" t="s">
         <v>10</v>
@@ -4809,45 +3345,9 @@
       <c r="V42" s="9">
         <v>1</v>
       </c>
-      <c r="W42" s="9">
-        <v>0</v>
-      </c>
-      <c r="X42" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH42" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:34">
-      <c r="B43" s="17"/>
+    </row>
+    <row r="43" spans="2:22">
+      <c r="B43" s="15"/>
       <c r="C43" s="13"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -4856,7 +3356,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="6">
-        <f t="shared" ref="G43:AH43" si="6">AVERAGE(G36:G42)</f>
+        <f t="shared" ref="G43:V43" si="6">AVERAGE(G36:G42)</f>
         <v>0</v>
       </c>
       <c r="H43" s="6">
@@ -4919,57 +3419,9 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="W43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AA43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AD43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AE43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AF43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AG43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AH43" s="6">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:34">
-      <c r="B44" s="17"/>
+    </row>
+    <row r="44" spans="2:22">
+      <c r="B44" s="15"/>
       <c r="C44" s="12" t="s">
         <v>47</v>
       </c>
@@ -5028,45 +3480,9 @@
       <c r="V44" s="9">
         <v>1</v>
       </c>
-      <c r="W44" s="9">
-        <v>0</v>
-      </c>
-      <c r="X44" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG44" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH44" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:34">
-      <c r="B45" s="17"/>
+    </row>
+    <row r="45" spans="2:22">
+      <c r="B45" s="15"/>
       <c r="C45" s="12"/>
       <c r="D45" s="7" t="s">
         <v>64</v>
@@ -5123,45 +3539,9 @@
       <c r="V45" s="9">
         <v>1</v>
       </c>
-      <c r="W45" s="9">
-        <v>0</v>
-      </c>
-      <c r="X45" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG45" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH45" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:34">
-      <c r="B46" s="18"/>
+    </row>
+    <row r="46" spans="2:22">
+      <c r="B46" s="16"/>
       <c r="C46" s="13"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -5170,7 +3550,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="6">
-        <f t="shared" ref="G46:AH46" si="7">AVERAGE(G44:G45)</f>
+        <f t="shared" ref="G46:V46" si="7">AVERAGE(G44:G45)</f>
         <v>0</v>
       </c>
       <c r="H46" s="6">
@@ -5233,57 +3613,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="W46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="X46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Z46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AA46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AD46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AE46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AF46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AG46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AH46" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:34">
-      <c r="B47" s="16" t="s">
+    </row>
+    <row r="47" spans="2:22">
+      <c r="B47" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -5344,45 +3676,9 @@
       <c r="V47" s="9">
         <v>1</v>
       </c>
-      <c r="W47" s="9">
-        <v>0</v>
-      </c>
-      <c r="X47" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG47" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH47" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:34">
-      <c r="B48" s="17"/>
+    </row>
+    <row r="48" spans="2:22">
+      <c r="B48" s="15"/>
       <c r="C48" s="12"/>
       <c r="D48" s="7" t="s">
         <v>25</v>
@@ -5439,45 +3735,9 @@
       <c r="V48" s="9">
         <v>1</v>
       </c>
-      <c r="W48" s="9">
-        <v>0</v>
-      </c>
-      <c r="X48" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG48" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH48" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:34">
-      <c r="B49" s="17"/>
+    </row>
+    <row r="49" spans="2:22">
+      <c r="B49" s="15"/>
       <c r="C49" s="12"/>
       <c r="D49" s="7" t="s">
         <v>26</v>
@@ -5534,45 +3794,9 @@
       <c r="V49" s="9">
         <v>1</v>
       </c>
-      <c r="W49" s="9">
-        <v>0</v>
-      </c>
-      <c r="X49" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG49" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH49" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:34">
-      <c r="B50" s="17"/>
+    </row>
+    <row r="50" spans="2:22">
+      <c r="B50" s="15"/>
       <c r="C50" s="12"/>
       <c r="D50" s="7" t="s">
         <v>27</v>
@@ -5629,45 +3853,9 @@
       <c r="V50" s="9">
         <v>1</v>
       </c>
-      <c r="W50" s="9">
-        <v>0</v>
-      </c>
-      <c r="X50" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG50" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH50" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:34">
-      <c r="B51" s="17"/>
+    </row>
+    <row r="51" spans="2:22">
+      <c r="B51" s="15"/>
       <c r="C51" s="12"/>
       <c r="D51" s="7" t="s">
         <v>15</v>
@@ -5724,45 +3912,9 @@
       <c r="V51" s="9">
         <v>1</v>
       </c>
-      <c r="W51" s="9">
-        <v>0</v>
-      </c>
-      <c r="X51" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG51" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH51" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:34">
-      <c r="B52" s="17"/>
+    </row>
+    <row r="52" spans="2:22">
+      <c r="B52" s="15"/>
       <c r="C52" s="12"/>
       <c r="D52" s="7" t="s">
         <v>16</v>
@@ -5819,45 +3971,9 @@
       <c r="V52" s="9">
         <v>1</v>
       </c>
-      <c r="W52" s="9">
-        <v>0</v>
-      </c>
-      <c r="X52" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG52" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH52" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:34">
-      <c r="B53" s="17"/>
+    </row>
+    <row r="53" spans="2:22">
+      <c r="B53" s="15"/>
       <c r="C53" s="12"/>
       <c r="D53" s="7" t="s">
         <v>28</v>
@@ -5914,45 +4030,9 @@
       <c r="V53" s="9">
         <v>1</v>
       </c>
-      <c r="W53" s="9">
-        <v>0</v>
-      </c>
-      <c r="X53" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG53" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH53" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:34">
-      <c r="B54" s="17"/>
+    </row>
+    <row r="54" spans="2:22">
+      <c r="B54" s="15"/>
       <c r="C54" s="12"/>
       <c r="D54" s="7" t="s">
         <v>29</v>
@@ -6009,45 +4089,9 @@
       <c r="V54" s="9">
         <v>1</v>
       </c>
-      <c r="W54" s="9">
-        <v>0</v>
-      </c>
-      <c r="X54" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG54" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH54" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:34">
-      <c r="B55" s="17"/>
+    </row>
+    <row r="55" spans="2:22">
+      <c r="B55" s="15"/>
       <c r="C55" s="12"/>
       <c r="D55" s="7" t="s">
         <v>67</v>
@@ -6084,45 +4128,9 @@
       <c r="V55" s="9">
         <v>1</v>
       </c>
-      <c r="W55" s="9">
-        <v>0</v>
-      </c>
-      <c r="X55" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG55" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH55" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:34">
-      <c r="B56" s="17"/>
+    </row>
+    <row r="56" spans="2:22">
+      <c r="B56" s="15"/>
       <c r="C56" s="12"/>
       <c r="D56" s="7" t="s">
         <v>66</v>
@@ -6179,45 +4187,9 @@
       <c r="V56" s="9">
         <v>1</v>
       </c>
-      <c r="W56" s="9">
-        <v>0</v>
-      </c>
-      <c r="X56" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG56" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH56" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:34">
-      <c r="B57" s="17"/>
+    </row>
+    <row r="57" spans="2:22">
+      <c r="B57" s="15"/>
       <c r="C57" s="12"/>
       <c r="D57" s="7" t="s">
         <v>30</v>
@@ -6274,45 +4246,9 @@
       <c r="V57" s="9">
         <v>1</v>
       </c>
-      <c r="W57" s="9">
-        <v>0</v>
-      </c>
-      <c r="X57" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG57" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH57" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:34">
-      <c r="B58" s="17"/>
+    </row>
+    <row r="58" spans="2:22">
+      <c r="B58" s="15"/>
       <c r="C58" s="12"/>
       <c r="D58" s="7" t="s">
         <v>31</v>
@@ -6369,45 +4305,9 @@
       <c r="V58" s="9">
         <v>1</v>
       </c>
-      <c r="W58" s="9">
-        <v>0</v>
-      </c>
-      <c r="X58" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG58" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH58" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:34">
-      <c r="B59" s="17"/>
+    </row>
+    <row r="59" spans="2:22">
+      <c r="B59" s="15"/>
       <c r="C59" s="12"/>
       <c r="D59" s="7" t="s">
         <v>32</v>
@@ -6464,45 +4364,9 @@
       <c r="V59" s="9">
         <v>1</v>
       </c>
-      <c r="W59" s="9">
-        <v>0</v>
-      </c>
-      <c r="X59" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG59" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH59" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:34">
-      <c r="B60" s="17"/>
+    </row>
+    <row r="60" spans="2:22">
+      <c r="B60" s="15"/>
       <c r="C60" s="12"/>
       <c r="D60" s="7" t="s">
         <v>33</v>
@@ -6559,50 +4423,14 @@
       <c r="V60" s="9">
         <v>1</v>
       </c>
-      <c r="W60" s="9">
-        <v>0</v>
-      </c>
-      <c r="X60" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG60" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH60" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:34">
-      <c r="B61" s="17"/>
+    </row>
+    <row r="61" spans="2:22">
+      <c r="B61" s="15"/>
       <c r="C61" s="13"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="6">
-        <f t="shared" ref="F61:AH61" si="8">AVERAGE(F47:F60)</f>
+        <f t="shared" ref="F61:V61" si="8">AVERAGE(F47:F60)</f>
         <v>0</v>
       </c>
       <c r="G61" s="6">
@@ -6669,58 +4497,10 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="W61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="X61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Y61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AD61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AE61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AF61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AG61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AH61" s="6">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B62" s="17"/>
-      <c r="C62" s="14" t="s">
+    </row>
+    <row r="62" spans="2:22" ht="16.5" customHeight="1">
+      <c r="B62" s="15"/>
+      <c r="C62" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="7" t="s">
@@ -6778,46 +4558,10 @@
       <c r="V62" s="9">
         <v>1</v>
       </c>
-      <c r="W62" s="9">
-        <v>0</v>
-      </c>
-      <c r="X62" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG62" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:34">
-      <c r="B63" s="17"/>
-      <c r="C63" s="15"/>
+    </row>
+    <row r="63" spans="2:22">
+      <c r="B63" s="15"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="6">
@@ -6825,7 +4569,7 @@
         <v>0</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" ref="G63:AH63" si="9">AVERAGE(G62)</f>
+        <f t="shared" ref="G63:V63" si="9">AVERAGE(G62)</f>
         <v>0</v>
       </c>
       <c r="H63" s="6">
@@ -6888,57 +4632,9 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="W63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="X63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Y63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="Z63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AA63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AB63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AC63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AD63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AE63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AF63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AG63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AH63" s="6">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:34">
-      <c r="B64" s="17"/>
+    </row>
+    <row r="64" spans="2:22">
+      <c r="B64" s="15"/>
       <c r="C64" s="11" t="s">
         <v>38</v>
       </c>
@@ -6997,45 +4693,9 @@
       <c r="V64" s="9">
         <v>1</v>
       </c>
-      <c r="W64" s="9">
-        <v>0</v>
-      </c>
-      <c r="X64" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG64" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH64" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:34">
-      <c r="B65" s="17"/>
+    </row>
+    <row r="65" spans="2:22">
+      <c r="B65" s="15"/>
       <c r="C65" s="13"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -7092,7 +4752,7 @@
         <v>1</v>
       </c>
       <c r="S65" s="6">
-        <f t="shared" ref="S65:AH65" si="11">AVERAGE(S64)</f>
+        <f t="shared" ref="S65:V65" si="11">AVERAGE(S64)</f>
         <v>1</v>
       </c>
       <c r="T65" s="6">
@@ -7107,57 +4767,9 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="W65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="X65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Y65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Z65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AA65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AD65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AE65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AF65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AG65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AH65" s="6">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:34" ht="16.5" customHeight="1">
-      <c r="B66" s="17"/>
+    </row>
+    <row r="66" spans="2:22" ht="16.5" customHeight="1">
+      <c r="B66" s="15"/>
       <c r="C66" s="11" t="s">
         <v>40</v>
       </c>
@@ -7216,45 +4828,9 @@
       <c r="V66" s="9">
         <v>1</v>
       </c>
-      <c r="W66" s="9">
-        <v>0</v>
-      </c>
-      <c r="X66" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG66" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH66" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:34">
-      <c r="B67" s="17"/>
+    </row>
+    <row r="67" spans="2:22">
+      <c r="B67" s="15"/>
       <c r="C67" s="12"/>
       <c r="D67" s="7" t="s">
         <v>37</v>
@@ -7311,45 +4887,9 @@
       <c r="V67" s="9">
         <v>1</v>
       </c>
-      <c r="W67" s="9">
-        <v>0</v>
-      </c>
-      <c r="X67" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AA67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AB67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG67" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH67" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:34">
-      <c r="B68" s="18"/>
+    </row>
+    <row r="68" spans="2:22">
+      <c r="B68" s="16"/>
       <c r="C68" s="13"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -7406,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="S68" s="6">
-        <f t="shared" ref="S68:AH68" si="13">AVERAGE(S66:S67)</f>
+        <f t="shared" ref="S68:V68" si="13">AVERAGE(S66:S67)</f>
         <v>1</v>
       </c>
       <c r="T68" s="6">
@@ -7421,60 +4961,12 @@
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
-      <c r="W68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="X68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Y68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="Z68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AA68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AB68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AC68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AD68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AE68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AF68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AG68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AH68" s="6">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:34">
+    </row>
+    <row r="69" spans="2:22">
       <c r="E69" s="8"/>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" spans="2:34">
+    <row r="70" spans="2:22">
       <c r="E70" s="8"/>
       <c r="F70" s="4"/>
     </row>
@@ -7694,48 +5186,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{65D6EC0D-952A-420C-9BCF-6E4C561DF568}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6:AH15">
-    <cfRule type="dataBar" priority="651">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BE0275C9-A13C-4221-B9B7-203BFE7719CD}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17:AH18">
-    <cfRule type="dataBar" priority="555">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A0E20ECF-5663-478F-8E9F-449195CDAA9F}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F62:AH62">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{CD51EF20-327A-4158-B3A7-ED5CFD3059B4}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8020,34 +5470,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:AH15">
-    <cfRule type="dataBar" priority="652">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{BC994E96-D1FB-4FF1-98B0-81DBE99950DE}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H45:AH45">
-    <cfRule type="dataBar" priority="501">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{5A887C91-57E6-4A6F-9712-7D026683BD38}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I22:I24">
     <cfRule type="dataBar" priority="10">
       <dataBar>
@@ -8132,20 +5554,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I44:AH44">
-    <cfRule type="dataBar" priority="19">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{196E49F1-0D91-4E01-BC7E-8AB3EB3E8E66}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J39:J42 K40:K42">
     <cfRule type="dataBar" priority="27">
       <dataBar>
@@ -8156,20 +5564,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{18153AA0-6BDF-4B6B-B2C4-171DA42A3821}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J48:J49 J50:AH60">
-    <cfRule type="dataBar" priority="562">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{90455EE3-E7AD-4F59-8325-47922778E0F6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -8216,8 +5610,106 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K36:O36 L40:O42 K38:O39 L37:O37 P36:AH42">
-    <cfRule type="dataBar" priority="18">
+  <conditionalFormatting sqref="F6:V15">
+    <cfRule type="dataBar" priority="653">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BE0275C9-A13C-4221-B9B7-203BFE7719CD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17:V18">
+    <cfRule type="dataBar" priority="654">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A0E20ECF-5663-478F-8E9F-449195CDAA9F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F62:V62">
+    <cfRule type="dataBar" priority="655">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{CD51EF20-327A-4158-B3A7-ED5CFD3059B4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:V15">
+    <cfRule type="dataBar" priority="656">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BC994E96-D1FB-4FF1-98B0-81DBE99950DE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:V45">
+    <cfRule type="dataBar" priority="657">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5A887C91-57E6-4A6F-9712-7D026683BD38}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44:V44">
+    <cfRule type="dataBar" priority="658">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{196E49F1-0D91-4E01-BC7E-8AB3EB3E8E66}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48:J49 J50:V60">
+    <cfRule type="dataBar" priority="659">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{90455EE3-E7AD-4F59-8325-47922778E0F6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K36:O36 L40:O42 K38:O39 L37:O37 P36:V42">
+    <cfRule type="dataBar" priority="661">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8230,8 +5722,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33:AH34">
-    <cfRule type="dataBar" priority="16">
+  <conditionalFormatting sqref="K33:V34">
+    <cfRule type="dataBar" priority="666">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8244,8 +5736,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K47:AH49">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="K47:V49">
+    <cfRule type="dataBar" priority="667">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8258,8 +5750,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20:AH24">
-    <cfRule type="dataBar" priority="25">
+  <conditionalFormatting sqref="L20:V24">
+    <cfRule type="dataBar" priority="668">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8272,8 +5764,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L64:AH64">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="L64:V64">
+    <cfRule type="dataBar" priority="669">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8286,8 +5778,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L66:AH67">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="L66:V67">
+    <cfRule type="dataBar" priority="670">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8300,8 +5792,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W26:AH32 K32:V32 K29:V29 L26:V28 L30:V31">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="K32:V32 K29:V29 L26:V28 L30:V31">
+    <cfRule type="dataBar" priority="671">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -8450,39 +5942,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>F64:I64 F44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BE0275C9-A13C-4221-B9B7-203BFE7719CD}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F6:AH15</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A0E20ECF-5663-478F-8E9F-449195CDAA9F}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F17:AH18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CD51EF20-327A-4158-B3A7-ED5CFD3059B4}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F62:AH62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{57A8B765-FFA7-434C-9523-5857F06016E6}">
@@ -8705,28 +6164,6 @@
           <xm:sqref>H66:K66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BC994E96-D1FB-4FF1-98B0-81DBE99950DE}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H6:AH15</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5A887C91-57E6-4A6F-9712-7D026683BD38}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H45:AH45</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1A303F07-6070-4189-AC1D-80357A0D5D47}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
@@ -8793,17 +6230,6 @@
           <xm:sqref>I67:K67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{196E49F1-0D91-4E01-BC7E-8AB3EB3E8E66}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>I44:AH44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{18153AA0-6BDF-4B6B-B2C4-171DA42A3821}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
@@ -8813,17 +6239,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>J39:J42 K40:K42</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{90455EE3-E7AD-4F59-8325-47922778E0F6}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>J48:J49 J50:AH60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{DBDB9E12-FBD7-4ED7-8AF2-CC272D920CAD}">
@@ -8859,6 +6274,83 @@
           <xm:sqref>J64:K64 J47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BE0275C9-A13C-4221-B9B7-203BFE7719CD}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F6:V15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A0E20ECF-5663-478F-8E9F-449195CDAA9F}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F17:V18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{CD51EF20-327A-4158-B3A7-ED5CFD3059B4}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F62:V62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BC994E96-D1FB-4FF1-98B0-81DBE99950DE}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H6:V15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5A887C91-57E6-4A6F-9712-7D026683BD38}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H45:V45</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{196E49F1-0D91-4E01-BC7E-8AB3EB3E8E66}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I44:V44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{90455EE3-E7AD-4F59-8325-47922778E0F6}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J48:J49 J50:V60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6C5573C3-41FA-4990-9C24-439EC153DA6C}">
             <x14:dataBar minLength="0" maxLength="100">
               <x14:cfvo type="autoMin"/>
@@ -8867,7 +6359,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K36:O36 L40:O42 K38:O39 L37:O37 P36:AH42</xm:sqref>
+          <xm:sqref>K36:O36 L40:O42 K38:O39 L37:O37 P36:V42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{79A6E942-BB28-4C5C-B051-63D2113FB72F}">
@@ -8878,7 +6370,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K33:AH34</xm:sqref>
+          <xm:sqref>K33:V34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{018A2B3E-2548-4772-A2CF-BD33006C0FDF}">
@@ -8889,7 +6381,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>K47:AH49</xm:sqref>
+          <xm:sqref>K47:V49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4C3D459D-49E3-462A-B846-0FE83B131D15}">
@@ -8900,7 +6392,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L20:AH24</xm:sqref>
+          <xm:sqref>L20:V24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{CBE33775-0E9E-48FA-B07E-81B3AA0F642B}">
@@ -8911,7 +6403,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L64:AH64</xm:sqref>
+          <xm:sqref>L64:V64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B769FDA4-52DD-48E5-B5B4-67E966D84479}">
@@ -8922,7 +6414,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>L66:AH67</xm:sqref>
+          <xm:sqref>L66:V67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{5D6CA6F3-5CED-49CB-9FFA-6686FDCC177F}">
@@ -8933,7 +6425,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>W26:AH32 K32:V32 K29:V29 L26:V28 L30:V31</xm:sqref>
+          <xm:sqref>K32:V32 K29:V29 L26:V28 L30:V31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>